<commit_message>
Made corrections to below after checking with Tableau, Freight now DONE
</commit_message>
<xml_diff>
--- a/input/WB1.xlsx
+++ b/input/WB1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DDPTemplateAutomationV2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51666A2D-02B4-413D-AC28-A91A0F322914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91FFB18-F451-4AFB-9612-FA71FCD58D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="888" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2788,7 +2788,7 @@
     <t>Freight CH4</t>
   </si>
   <si>
-    <t>mt</t>
+    <t>kt</t>
   </si>
   <si>
     <t>Freight N2O</t>
@@ -6413,6 +6413,8 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="2" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -6458,8 +6460,6 @@
     <xf numFmtId="0" fontId="47" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="5x indented GHG Textfiels" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -8331,23 +8331,23 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:17" ht="268.5" customHeight="1">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="225"/>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="225"/>
-      <c r="J4" s="225"/>
-      <c r="K4" s="225"/>
-      <c r="L4" s="225"/>
-      <c r="M4" s="225"/>
-      <c r="N4" s="225"/>
-      <c r="O4" s="226"/>
+      <c r="B4" s="227"/>
+      <c r="C4" s="227"/>
+      <c r="D4" s="227"/>
+      <c r="E4" s="227"/>
+      <c r="F4" s="227"/>
+      <c r="G4" s="227"/>
+      <c r="H4" s="227"/>
+      <c r="I4" s="227"/>
+      <c r="J4" s="227"/>
+      <c r="K4" s="227"/>
+      <c r="L4" s="227"/>
+      <c r="M4" s="227"/>
+      <c r="N4" s="227"/>
+      <c r="O4" s="228"/>
       <c r="Q4" s="177"/>
     </row>
     <row r="5" spans="1:17">
@@ -8368,23 +8368,23 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:17" ht="289.5" customHeight="1">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="225"/>
-      <c r="C6" s="225"/>
-      <c r="D6" s="225"/>
-      <c r="E6" s="225"/>
-      <c r="F6" s="225"/>
-      <c r="G6" s="225"/>
-      <c r="H6" s="225"/>
-      <c r="I6" s="225"/>
-      <c r="J6" s="225"/>
-      <c r="K6" s="225"/>
-      <c r="L6" s="225"/>
-      <c r="M6" s="225"/>
-      <c r="N6" s="225"/>
-      <c r="O6" s="226"/>
+      <c r="B6" s="227"/>
+      <c r="C6" s="227"/>
+      <c r="D6" s="227"/>
+      <c r="E6" s="227"/>
+      <c r="F6" s="227"/>
+      <c r="G6" s="227"/>
+      <c r="H6" s="227"/>
+      <c r="I6" s="227"/>
+      <c r="J6" s="227"/>
+      <c r="K6" s="227"/>
+      <c r="L6" s="227"/>
+      <c r="M6" s="227"/>
+      <c r="N6" s="227"/>
+      <c r="O6" s="228"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="5"/>
@@ -8421,23 +8421,23 @@
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:17" ht="21" customHeight="1">
-      <c r="A9" s="227" t="s">
+      <c r="A9" s="229" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="228"/>
-      <c r="C9" s="228"/>
-      <c r="D9" s="228"/>
-      <c r="E9" s="228"/>
-      <c r="F9" s="228"/>
-      <c r="G9" s="228"/>
-      <c r="H9" s="228"/>
-      <c r="I9" s="228"/>
-      <c r="J9" s="228"/>
-      <c r="K9" s="228"/>
-      <c r="L9" s="228"/>
-      <c r="M9" s="228"/>
-      <c r="N9" s="228"/>
-      <c r="O9" s="229"/>
+      <c r="B9" s="230"/>
+      <c r="C9" s="230"/>
+      <c r="D9" s="230"/>
+      <c r="E9" s="230"/>
+      <c r="F9" s="230"/>
+      <c r="G9" s="230"/>
+      <c r="H9" s="230"/>
+      <c r="I9" s="230"/>
+      <c r="J9" s="230"/>
+      <c r="K9" s="230"/>
+      <c r="L9" s="230"/>
+      <c r="M9" s="230"/>
+      <c r="N9" s="230"/>
+      <c r="O9" s="231"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="148"/>
@@ -8807,23 +8807,23 @@
       <c r="O28" s="7"/>
     </row>
     <row r="29" spans="1:15" ht="54" customHeight="1">
-      <c r="A29" s="217" t="s">
+      <c r="A29" s="219" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="218"/>
-      <c r="C29" s="218"/>
-      <c r="D29" s="218"/>
-      <c r="E29" s="218"/>
-      <c r="F29" s="218"/>
-      <c r="G29" s="218"/>
-      <c r="H29" s="218"/>
-      <c r="I29" s="218"/>
-      <c r="J29" s="218"/>
-      <c r="K29" s="218"/>
-      <c r="L29" s="218"/>
-      <c r="M29" s="218"/>
-      <c r="N29" s="218"/>
-      <c r="O29" s="219"/>
+      <c r="B29" s="220"/>
+      <c r="C29" s="220"/>
+      <c r="D29" s="220"/>
+      <c r="E29" s="220"/>
+      <c r="F29" s="220"/>
+      <c r="G29" s="220"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="220"/>
+      <c r="J29" s="220"/>
+      <c r="K29" s="220"/>
+      <c r="L29" s="220"/>
+      <c r="M29" s="220"/>
+      <c r="N29" s="220"/>
+      <c r="O29" s="221"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="9"/>
@@ -8881,23 +8881,23 @@
       <c r="O32" s="7"/>
     </row>
     <row r="33" spans="1:15" ht="60" customHeight="1">
-      <c r="A33" s="217" t="s">
+      <c r="A33" s="219" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="218"/>
-      <c r="C33" s="218"/>
-      <c r="D33" s="218"/>
-      <c r="E33" s="218"/>
-      <c r="F33" s="218"/>
-      <c r="G33" s="218"/>
-      <c r="H33" s="218"/>
-      <c r="I33" s="218"/>
-      <c r="J33" s="218"/>
-      <c r="K33" s="218"/>
-      <c r="L33" s="218"/>
-      <c r="M33" s="218"/>
-      <c r="N33" s="218"/>
-      <c r="O33" s="219"/>
+      <c r="B33" s="220"/>
+      <c r="C33" s="220"/>
+      <c r="D33" s="220"/>
+      <c r="E33" s="220"/>
+      <c r="F33" s="220"/>
+      <c r="G33" s="220"/>
+      <c r="H33" s="220"/>
+      <c r="I33" s="220"/>
+      <c r="J33" s="220"/>
+      <c r="K33" s="220"/>
+      <c r="L33" s="220"/>
+      <c r="M33" s="220"/>
+      <c r="N33" s="220"/>
+      <c r="O33" s="221"/>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="145"/>
@@ -8950,7 +8950,7 @@
       </c>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="220" t="s">
+      <c r="A39" s="222" t="s">
         <v>29</v>
       </c>
       <c r="B39" s="173" t="s">
@@ -8961,7 +8961,7 @@
       </c>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="221"/>
+      <c r="A40" s="223"/>
       <c r="B40" s="173" t="s">
         <v>31</v>
       </c>
@@ -8970,7 +8970,7 @@
       </c>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="222"/>
+      <c r="A41" s="224"/>
       <c r="B41" s="173" t="s">
         <v>32</v>
       </c>
@@ -8979,7 +8979,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A42" s="223" t="s">
+      <c r="A42" s="225" t="s">
         <v>34</v>
       </c>
       <c r="B42" s="174" t="s">
@@ -8990,7 +8990,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A43" s="221"/>
+      <c r="A43" s="223"/>
       <c r="B43" s="174" t="s">
         <v>37</v>
       </c>
@@ -8999,7 +8999,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A44" s="221"/>
+      <c r="A44" s="223"/>
       <c r="B44" s="174" t="s">
         <v>39</v>
       </c>
@@ -9008,7 +9008,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A45" s="221"/>
+      <c r="A45" s="223"/>
       <c r="B45" s="174" t="s">
         <v>41</v>
       </c>
@@ -9017,7 +9017,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A46" s="221"/>
+      <c r="A46" s="223"/>
       <c r="B46" s="174" t="s">
         <v>43</v>
       </c>
@@ -9026,7 +9026,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A47" s="221"/>
+      <c r="A47" s="223"/>
       <c r="B47" s="174" t="s">
         <v>45</v>
       </c>
@@ -9035,7 +9035,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A48" s="221"/>
+      <c r="A48" s="223"/>
       <c r="B48" s="174" t="s">
         <v>47</v>
       </c>
@@ -9044,7 +9044,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A49" s="221"/>
+      <c r="A49" s="223"/>
       <c r="B49" s="174" t="s">
         <v>49</v>
       </c>
@@ -9053,7 +9053,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A50" s="221"/>
+      <c r="A50" s="223"/>
       <c r="B50" s="174" t="s">
         <v>50</v>
       </c>
@@ -9062,7 +9062,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A51" s="222"/>
+      <c r="A51" s="224"/>
       <c r="B51" s="174" t="s">
         <v>52</v>
       </c>
@@ -9095,8 +9095,8 @@
   </sheetPr>
   <dimension ref="A1:L259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:G22"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179:G180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9234,15 +9234,15 @@
       </c>
       <c r="E8" s="166">
         <f t="shared" si="1"/>
-        <v>1.2472587705342659</v>
+        <v>1.0895711879257897</v>
       </c>
       <c r="F8" s="166">
         <f t="shared" si="1"/>
-        <v>1.0730322135032291</v>
+        <v>0.89953589065139072</v>
       </c>
       <c r="G8" s="166">
         <f t="shared" si="1"/>
-        <v>0.42413657533377291</v>
+        <v>0.36616102091648722</v>
       </c>
       <c r="H8" s="166" t="e">
         <f t="shared" si="1"/>
@@ -9270,11 +9270,11 @@
       </c>
       <c r="E9" s="166">
         <f t="shared" si="2"/>
-        <v>68.952953347573242</v>
+        <v>66.710370955960542</v>
       </c>
       <c r="F9" s="166">
         <f t="shared" si="2"/>
-        <v>64.0267432321575</v>
+        <v>60.878289723330155</v>
       </c>
       <c r="G9" s="166">
         <f t="shared" si="2"/>
@@ -9306,15 +9306,15 @@
       </c>
       <c r="E10" s="166">
         <f t="shared" si="3"/>
-        <v>418.54200000000003</v>
+        <v>432.61200000000002</v>
       </c>
       <c r="F10" s="166">
         <f t="shared" si="3"/>
-        <v>451.03</v>
+        <v>474.35599999999999</v>
       </c>
       <c r="G10" s="166">
         <f t="shared" si="3"/>
-        <v>223.154</v>
+        <v>257.25</v>
       </c>
       <c r="H10" s="166">
         <f t="shared" si="3"/>
@@ -9374,15 +9374,15 @@
       </c>
       <c r="D12" s="166">
         <f t="shared" si="5"/>
-        <v>18.624108</v>
+        <v>0.10173</v>
       </c>
       <c r="E12" s="166">
         <f t="shared" si="5"/>
-        <v>17.775507000000001</v>
+        <v>9.7095000000000001E-2</v>
       </c>
       <c r="F12" s="166">
         <f t="shared" si="5"/>
-        <v>17.513341999999998</v>
+        <v>9.5662999999999998E-2</v>
       </c>
       <c r="G12" s="166">
         <f t="shared" si="5"/>
@@ -9618,16 +9618,16 @@
         <v>5690330.8418548107</v>
       </c>
       <c r="E22" s="39">
-        <f t="shared" ref="E22:G22" si="7">E252*E253*1000</f>
-        <v>5654432.8749407493</v>
+        <f>E252*E253*1000</f>
+        <v>6656608.237284435</v>
       </c>
       <c r="F22" s="39">
-        <f t="shared" si="7"/>
-        <v>5499004.8067556117</v>
+        <f>F252*F253*1000</f>
+        <v>6939321.8357880721</v>
       </c>
       <c r="G22" s="39">
-        <f t="shared" si="7"/>
-        <v>8438282.9703348428</v>
+        <f>G252*G253*1000</f>
+        <v>11293466.453526629</v>
       </c>
       <c r="H22" s="55"/>
       <c r="I22" s="55"/>
@@ -9647,13 +9647,13 @@
         <v>350.9537072498461</v>
       </c>
       <c r="E23" s="210">
-        <v>335.56949839744698</v>
+        <v>397.04794399305013</v>
       </c>
       <c r="F23" s="210">
-        <v>420.33220841290489</v>
+        <v>527.33415634644598</v>
       </c>
       <c r="G23" s="210">
-        <v>526.13712888210523</v>
+        <v>702.55976279537595</v>
       </c>
       <c r="H23" s="55"/>
       <c r="I23" s="55"/>
@@ -10004,20 +10004,20 @@
       </c>
       <c r="C43" s="55"/>
       <c r="D43" s="39">
-        <f t="shared" ref="D43:G44" si="8">D$23*D254</f>
+        <f t="shared" ref="D43:G44" si="7">D$23*D254</f>
         <v>236.19835508164178</v>
       </c>
       <c r="E43" s="39">
-        <f t="shared" si="8"/>
-        <v>240.94256282751797</v>
+        <f t="shared" si="7"/>
+        <v>285.08475784582856</v>
       </c>
       <c r="F43" s="39">
-        <f t="shared" si="8"/>
-        <v>317.33962890685694</v>
+        <f t="shared" si="7"/>
+        <v>398.12325140809719</v>
       </c>
       <c r="G43" s="39">
-        <f t="shared" si="8"/>
-        <v>415.64275833032838</v>
+        <f t="shared" si="7"/>
+        <v>555.01477023797838</v>
       </c>
       <c r="H43" s="55"/>
       <c r="I43" s="55"/>
@@ -10034,20 +10034,20 @@
       </c>
       <c r="C44" s="55"/>
       <c r="D44" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>114.75535216820433</v>
       </c>
       <c r="E44" s="39">
-        <f t="shared" si="8"/>
-        <v>94.626935569928989</v>
+        <f t="shared" si="7"/>
+        <v>111.96318614722158</v>
       </c>
       <c r="F44" s="39">
-        <f t="shared" si="8"/>
-        <v>102.99257950604796</v>
+        <f t="shared" si="7"/>
+        <v>129.21090493834879</v>
       </c>
       <c r="G44" s="39">
-        <f t="shared" si="8"/>
-        <v>110.49437055177687</v>
+        <f t="shared" si="7"/>
+        <v>147.54499255739756</v>
       </c>
       <c r="H44" s="55"/>
       <c r="I44" s="55"/>
@@ -10099,13 +10099,13 @@
         <v>223.47661800701411</v>
       </c>
       <c r="E47" s="211">
-        <v>187.39748219373851</v>
+        <v>248.87592778934149</v>
       </c>
       <c r="F47" s="211">
-        <v>226.6226500683299</v>
+        <v>333.62459800187088</v>
       </c>
       <c r="G47" s="211">
-        <v>269.47232742766892</v>
+        <v>445.89496134093957</v>
       </c>
       <c r="H47" s="55"/>
       <c r="I47" s="55"/>
@@ -10509,15 +10509,15 @@
       </c>
       <c r="E69" s="212">
         <f>E$47*E$254</f>
-        <v>134.55343779101659</v>
+        <v>178.69563280932704</v>
       </c>
       <c r="F69" s="212">
         <f>F$47*F$254</f>
-        <v>171.09406853715745</v>
+        <v>251.87769103839764</v>
       </c>
       <c r="G69" s="212">
         <f>G$47*G$254</f>
-        <v>212.88028408811874</v>
+        <v>352.25229599576875</v>
       </c>
       <c r="H69" s="99"/>
       <c r="I69" s="99"/>
@@ -10623,15 +10623,15 @@
       </c>
       <c r="E74" s="212">
         <f>E$47*E$255</f>
-        <v>52.84404440272192</v>
+        <v>70.180294980014452</v>
       </c>
       <c r="F74" s="212">
         <f>F$47*F$255</f>
-        <v>55.528581531172435</v>
+        <v>81.746906963473222</v>
       </c>
       <c r="G74" s="212">
         <f>G$47*G$255</f>
-        <v>56.592043339550173</v>
+        <v>93.64266534517084</v>
       </c>
       <c r="H74" s="55"/>
       <c r="I74" s="55"/>
@@ -10751,13 +10751,13 @@
         <v>205.0221467975187</v>
       </c>
       <c r="E80" s="210">
-        <v>166.44814684329091</v>
+        <v>227.926592438894</v>
       </c>
       <c r="F80" s="210">
-        <v>198.53952589163021</v>
+        <v>305.54147382517118</v>
       </c>
       <c r="G80" s="210">
-        <v>231.93875333241559</v>
+        <v>408.36138724568627</v>
       </c>
       <c r="H80" s="55"/>
       <c r="I80" s="55"/>
@@ -10803,13 +10803,13 @@
         <v>18.161092434957531</v>
       </c>
       <c r="E82" s="210">
-        <v>17.220374878361461</v>
+        <v>20.369760136126519</v>
       </c>
       <c r="F82" s="210">
-        <v>21.824749528074889</v>
+        <v>27.306188658639691</v>
       </c>
       <c r="G82" s="210">
-        <v>27.252546777996521</v>
+        <v>36.495186533710751</v>
       </c>
       <c r="H82" s="55"/>
       <c r="I82" s="55"/>
@@ -10961,15 +10961,15 @@
       </c>
       <c r="E90" s="39">
         <f>E$82*E$254</f>
-        <v>12.364417135221327</v>
+        <v>14.625710128061732</v>
       </c>
       <c r="F90" s="39">
         <f>F$82*F$254</f>
-        <v>16.477104960324404</v>
+        <v>20.615445598404218</v>
       </c>
       <c r="G90" s="39">
         <f>G$82*G$254</f>
-        <v>21.529223262384434</v>
+        <v>28.830810760079228</v>
       </c>
       <c r="H90" s="55"/>
       <c r="I90" s="55"/>
@@ -10991,15 +10991,15 @@
       </c>
       <c r="E91" s="39">
         <f>E$82*E$255</f>
-        <v>4.8559577431401353</v>
+        <v>5.7440500080647876</v>
       </c>
       <c r="F91" s="39">
         <f>F$82*F$255</f>
-        <v>5.3476445677504856</v>
+        <v>6.6907430602354721</v>
       </c>
       <c r="G91" s="39">
         <f>G$82*G$255</f>
-        <v>5.7233235156120879</v>
+        <v>7.6643757736315221</v>
       </c>
       <c r="H91" s="55"/>
       <c r="I91" s="55"/>
@@ -11095,13 +11095,13 @@
         <v>436.54866309996208</v>
       </c>
       <c r="E95" s="210">
-        <v>470.09792049886471</v>
+        <v>504.36209617242508</v>
       </c>
       <c r="F95" s="210">
-        <v>479.707556923906</v>
+        <v>573.79314341779332</v>
       </c>
       <c r="G95" s="210">
-        <v>723.92276161813868</v>
+        <v>886.32480565414153</v>
       </c>
       <c r="H95" s="55"/>
       <c r="I95" s="55"/>
@@ -11117,10 +11117,18 @@
         <v>728</v>
       </c>
       <c r="C96" s="55"/>
-      <c r="D96" s="210"/>
-      <c r="E96" s="210"/>
-      <c r="F96" s="210"/>
-      <c r="G96" s="210"/>
+      <c r="D96" s="210">
+        <v>10.16250289813785</v>
+      </c>
+      <c r="E96" s="210">
+        <v>25.690899789332821</v>
+      </c>
+      <c r="F96" s="210">
+        <v>36.090655825504179</v>
+      </c>
+      <c r="G96" s="210">
+        <v>112.67102499106809</v>
+      </c>
       <c r="H96" s="55"/>
       <c r="I96" s="55"/>
       <c r="J96" s="51"/>
@@ -11161,10 +11169,18 @@
         <v>728</v>
       </c>
       <c r="C98" s="55"/>
-      <c r="D98" s="210"/>
-      <c r="E98" s="210"/>
-      <c r="F98" s="210"/>
-      <c r="G98" s="210"/>
+      <c r="D98" s="210">
+        <v>84.767825491947093</v>
+      </c>
+      <c r="E98" s="210">
+        <v>127.056681225548</v>
+      </c>
+      <c r="F98" s="210">
+        <v>202.198323037595</v>
+      </c>
+      <c r="G98" s="210">
+        <v>621.02572732610702</v>
+      </c>
       <c r="H98" s="55"/>
       <c r="I98" s="55"/>
       <c r="J98" s="51"/>
@@ -11241,13 +11257,13 @@
       <c r="C102" s="55"/>
       <c r="D102" s="210"/>
       <c r="E102" s="210">
-        <v>22.129540309735301</v>
+        <v>56.393715983295813</v>
       </c>
       <c r="F102" s="210">
-        <v>91.929227611164848</v>
+        <v>186.01481410505221</v>
       </c>
       <c r="G102" s="210">
-        <v>399.32789522247913</v>
+        <v>561.72993925848198</v>
       </c>
       <c r="H102" s="55"/>
       <c r="I102" s="55"/>
@@ -11319,9 +11335,15 @@
         <v>728</v>
       </c>
       <c r="C106" s="55"/>
-      <c r="D106" s="210"/>
-      <c r="E106" s="210"/>
-      <c r="F106" s="210"/>
+      <c r="D106" s="210">
+        <v>10.16250289813785</v>
+      </c>
+      <c r="E106" s="210">
+        <v>14.08220962979731</v>
+      </c>
+      <c r="F106" s="210">
+        <v>13.1946672876697</v>
+      </c>
       <c r="G106" s="210"/>
       <c r="H106" s="55"/>
       <c r="I106" s="55"/>
@@ -11356,9 +11378,15 @@
       </c>
       <c r="C108" s="55"/>
       <c r="D108" s="210"/>
-      <c r="E108" s="210"/>
-      <c r="F108" s="210"/>
-      <c r="G108" s="210"/>
+      <c r="E108" s="210">
+        <v>11.608690159535509</v>
+      </c>
+      <c r="F108" s="210">
+        <v>16.802677804423091</v>
+      </c>
+      <c r="G108" s="210">
+        <v>79.791292948176491</v>
+      </c>
       <c r="H108" s="55"/>
       <c r="I108" s="55"/>
       <c r="J108" s="51"/>
@@ -11393,8 +11421,12 @@
       <c r="C110" s="55"/>
       <c r="D110" s="210"/>
       <c r="E110" s="210"/>
-      <c r="F110" s="210"/>
-      <c r="G110" s="210"/>
+      <c r="F110" s="210">
+        <v>6.0933107334113936</v>
+      </c>
+      <c r="G110" s="210">
+        <v>32.879732042891618</v>
+      </c>
       <c r="H110" s="55"/>
       <c r="I110" s="55"/>
       <c r="J110" s="51"/>
@@ -11543,9 +11575,15 @@
         <v>728</v>
       </c>
       <c r="C118" s="55"/>
-      <c r="D118" s="210"/>
-      <c r="E118" s="210"/>
-      <c r="F118" s="210"/>
+      <c r="D118" s="210">
+        <v>84.767825491947093</v>
+      </c>
+      <c r="E118" s="210">
+        <v>127.056681225548</v>
+      </c>
+      <c r="F118" s="210">
+        <v>101.967745722711</v>
+      </c>
       <c r="G118" s="210"/>
       <c r="H118" s="55"/>
       <c r="I118" s="55"/>
@@ -11581,8 +11619,12 @@
       <c r="C120" s="55"/>
       <c r="D120" s="210"/>
       <c r="E120" s="210"/>
-      <c r="F120" s="210"/>
-      <c r="G120" s="210"/>
+      <c r="F120" s="210">
+        <v>100.230577314884</v>
+      </c>
+      <c r="G120" s="210">
+        <v>621.02572732610702</v>
+      </c>
       <c r="H120" s="55"/>
       <c r="I120" s="55"/>
       <c r="J120" s="51"/>
@@ -11701,17 +11743,17 @@
         <v>238</v>
       </c>
       <c r="C127" s="60"/>
-      <c r="D127" s="238">
+      <c r="D127" s="217">
         <v>0.42794300000000002</v>
       </c>
-      <c r="E127" s="238">
-        <v>0.41854200000000003</v>
-      </c>
-      <c r="F127" s="238">
-        <v>0.45102999999999999</v>
-      </c>
-      <c r="G127" s="238">
-        <v>0.22315399999999999</v>
+      <c r="E127" s="217">
+        <v>0.432612</v>
+      </c>
+      <c r="F127" s="217">
+        <v>0.474356</v>
+      </c>
+      <c r="G127" s="217">
+        <v>0.25724999999999998</v>
       </c>
       <c r="H127" s="60"/>
       <c r="I127" s="60"/>
@@ -11725,10 +11767,10 @@
       </c>
       <c r="B128" s="98"/>
       <c r="C128" s="98"/>
-      <c r="D128" s="239"/>
-      <c r="E128" s="239"/>
-      <c r="F128" s="239"/>
-      <c r="G128" s="239"/>
+      <c r="D128" s="218"/>
+      <c r="E128" s="218"/>
+      <c r="F128" s="218"/>
+      <c r="G128" s="218"/>
       <c r="H128" s="98"/>
       <c r="I128" s="98"/>
       <c r="J128" s="51"/>
@@ -11743,17 +11785,17 @@
         <v>238</v>
       </c>
       <c r="C129" s="55"/>
-      <c r="D129" s="238">
+      <c r="D129" s="217">
         <v>0.41484700000000002</v>
       </c>
-      <c r="E129" s="238">
-        <v>0.40091500000000002</v>
-      </c>
-      <c r="F129" s="238">
-        <v>0.42044199999999998</v>
-      </c>
-      <c r="G129" s="238">
-        <v>0.17693900000000001</v>
+      <c r="E129" s="217">
+        <v>0.41498600000000002</v>
+      </c>
+      <c r="F129" s="217">
+        <v>0.44376700000000002</v>
+      </c>
+      <c r="G129" s="217">
+        <v>0.211035</v>
       </c>
       <c r="H129" s="55"/>
       <c r="I129" s="55"/>
@@ -11769,16 +11811,16 @@
         <v>238</v>
       </c>
       <c r="C130" s="55"/>
-      <c r="D130" s="238">
+      <c r="D130" s="217">
         <v>1.3096E-2</v>
       </c>
-      <c r="E130" s="238">
+      <c r="E130" s="217">
         <v>1.7627E-2</v>
       </c>
-      <c r="F130" s="238">
+      <c r="F130" s="217">
         <v>3.0588000000000001E-2</v>
       </c>
-      <c r="G130" s="238">
+      <c r="G130" s="217">
         <v>4.6216E-2</v>
       </c>
       <c r="H130" s="55"/>
@@ -11847,10 +11889,10 @@
       </c>
       <c r="B134" s="98"/>
       <c r="C134" s="98"/>
-      <c r="D134" s="239"/>
-      <c r="E134" s="239"/>
-      <c r="F134" s="239"/>
-      <c r="G134" s="239"/>
+      <c r="D134" s="218"/>
+      <c r="E134" s="218"/>
+      <c r="F134" s="218"/>
+      <c r="G134" s="218"/>
       <c r="H134" s="98"/>
       <c r="I134" s="98"/>
       <c r="J134" s="51"/>
@@ -11865,16 +11907,16 @@
         <v>238</v>
       </c>
       <c r="C135" s="55"/>
-      <c r="D135" s="238">
+      <c r="D135" s="217">
         <v>0.202876</v>
       </c>
-      <c r="E135" s="238">
+      <c r="E135" s="217">
         <v>0.160357</v>
       </c>
-      <c r="F135" s="238">
+      <c r="F135" s="217">
         <v>0.14983399999999999</v>
       </c>
-      <c r="G135" s="238"/>
+      <c r="G135" s="217"/>
       <c r="H135" s="55"/>
       <c r="I135" s="55"/>
       <c r="J135" s="51"/>
@@ -11907,15 +11949,15 @@
         <v>238</v>
       </c>
       <c r="C137" s="55"/>
-      <c r="D137" s="238"/>
-      <c r="E137" s="238">
-        <v>4.0020000000000003E-3</v>
-      </c>
-      <c r="F137" s="238">
-        <v>1.1445E-2</v>
-      </c>
-      <c r="G137" s="238">
-        <v>2.7816E-2</v>
+      <c r="D137" s="217"/>
+      <c r="E137" s="217">
+        <v>1.8072000000000001E-2</v>
+      </c>
+      <c r="F137" s="217">
+        <v>3.4770000000000002E-2</v>
+      </c>
+      <c r="G137" s="217">
+        <v>6.1912000000000002E-2</v>
       </c>
       <c r="H137" s="55"/>
       <c r="I137" s="55"/>
@@ -11967,12 +12009,12 @@
         <v>238</v>
       </c>
       <c r="C140" s="55"/>
-      <c r="D140" s="238"/>
-      <c r="E140" s="238"/>
-      <c r="F140" s="238">
+      <c r="D140" s="217"/>
+      <c r="E140" s="217"/>
+      <c r="F140" s="217">
         <v>5.3540000000000003E-3</v>
       </c>
-      <c r="G140" s="238">
+      <c r="G140" s="217">
         <v>5.7971000000000002E-2</v>
       </c>
       <c r="H140" s="55"/>
@@ -11989,16 +12031,16 @@
         <v>238</v>
       </c>
       <c r="C141" s="55"/>
-      <c r="D141" s="238">
+      <c r="D141" s="217">
         <v>0.202876</v>
       </c>
-      <c r="E141" s="238">
+      <c r="E141" s="217">
         <v>0.160357</v>
       </c>
-      <c r="F141" s="238">
+      <c r="F141" s="217">
         <v>0.14983399999999999</v>
       </c>
-      <c r="G141" s="238"/>
+      <c r="G141" s="217"/>
       <c r="H141" s="55"/>
       <c r="I141" s="55"/>
       <c r="J141" s="51"/>
@@ -12031,15 +12073,15 @@
         <v>238</v>
       </c>
       <c r="C143" s="55"/>
-      <c r="D143" s="238"/>
-      <c r="E143" s="238">
-        <v>4.0020000000000003E-3</v>
-      </c>
-      <c r="F143" s="238">
-        <v>1.1445E-2</v>
-      </c>
-      <c r="G143" s="238">
-        <v>2.7816E-2</v>
+      <c r="D143" s="217"/>
+      <c r="E143" s="217">
+        <v>1.8072000000000001E-2</v>
+      </c>
+      <c r="F143" s="217">
+        <v>3.4770000000000002E-2</v>
+      </c>
+      <c r="G143" s="217">
+        <v>6.1912000000000002E-2</v>
       </c>
       <c r="H143" s="55"/>
       <c r="I143" s="55"/>
@@ -12091,12 +12133,12 @@
         <v>238</v>
       </c>
       <c r="C146" s="55"/>
-      <c r="D146" s="238"/>
-      <c r="E146" s="238"/>
-      <c r="F146" s="238">
+      <c r="D146" s="217"/>
+      <c r="E146" s="217"/>
+      <c r="F146" s="217">
         <v>5.3540000000000003E-3</v>
       </c>
-      <c r="G146" s="238">
+      <c r="G146" s="217">
         <v>5.7971000000000002E-2</v>
       </c>
       <c r="H146" s="55"/>
@@ -12111,10 +12153,10 @@
       </c>
       <c r="B147" s="98"/>
       <c r="C147" s="98"/>
-      <c r="D147" s="239"/>
-      <c r="E147" s="239"/>
-      <c r="F147" s="239"/>
-      <c r="G147" s="239"/>
+      <c r="D147" s="218"/>
+      <c r="E147" s="218"/>
+      <c r="F147" s="218"/>
+      <c r="G147" s="218"/>
       <c r="H147" s="98"/>
       <c r="I147" s="98"/>
       <c r="J147" s="51"/>
@@ -12129,16 +12171,16 @@
         <v>238</v>
       </c>
       <c r="C148" s="60"/>
-      <c r="D148" s="238">
+      <c r="D148" s="217">
         <v>0.41864299999999999</v>
       </c>
-      <c r="E148" s="238">
+      <c r="E148" s="217">
         <v>0.39956700000000001</v>
       </c>
-      <c r="F148" s="238">
+      <c r="F148" s="217">
         <v>0.393673</v>
       </c>
-      <c r="G148" s="238"/>
+      <c r="G148" s="217"/>
       <c r="H148" s="60"/>
       <c r="I148" s="60"/>
       <c r="J148" s="51"/>
@@ -12207,17 +12249,17 @@
         <v>238</v>
       </c>
       <c r="C152" s="60"/>
-      <c r="D152" s="238">
+      <c r="D152" s="217">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="E152" s="238">
-        <v>1.8974000000000001E-2</v>
-      </c>
-      <c r="F152" s="238">
-        <v>5.2003000000000001E-2</v>
-      </c>
-      <c r="G152" s="238">
-        <v>0.165183</v>
+      <c r="E152" s="217">
+        <v>3.3044999999999998E-2</v>
+      </c>
+      <c r="F152" s="217">
+        <v>7.5328000000000006E-2</v>
+      </c>
+      <c r="G152" s="217">
+        <v>0.19927900000000001</v>
       </c>
       <c r="H152" s="60"/>
       <c r="I152" s="60"/>
@@ -12233,12 +12275,12 @@
         <v>238</v>
       </c>
       <c r="C153" s="60"/>
-      <c r="D153" s="238"/>
-      <c r="E153" s="238"/>
-      <c r="F153" s="238">
+      <c r="D153" s="217"/>
+      <c r="E153" s="217"/>
+      <c r="F153" s="217">
         <v>5.3540000000000003E-3</v>
       </c>
-      <c r="G153" s="238">
+      <c r="G153" s="217">
         <v>5.7971000000000002E-2</v>
       </c>
       <c r="H153" s="60"/>
@@ -12736,19 +12778,19 @@
       </c>
       <c r="C179" s="78"/>
       <c r="D179" s="216">
-        <f>28*D256+265*D257</f>
-        <v>18.624108</v>
+        <f>D256+D257</f>
+        <v>0.10173</v>
       </c>
       <c r="E179" s="216">
-        <f>28*E256+265*E257</f>
-        <v>17.775507000000001</v>
+        <f t="shared" ref="E179:G179" si="8">E256+E257</f>
+        <v>9.7095000000000001E-2</v>
       </c>
       <c r="F179" s="216">
-        <f>28*F256+265*F257</f>
-        <v>17.513341999999998</v>
+        <f t="shared" si="8"/>
+        <v>9.5662999999999998E-2</v>
       </c>
       <c r="G179" s="216">
-        <f>28*G256+265*G257</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H179" s="78"/>
@@ -12766,19 +12808,19 @@
       </c>
       <c r="C180" s="78"/>
       <c r="D180" s="216">
-        <f>28*D258+265*D259</f>
-        <v>9.0252809999999997</v>
+        <f>D258+D259</f>
+        <v>4.9299000000000003E-2</v>
       </c>
       <c r="E180" s="216">
-        <f>28*E258+265*E259</f>
-        <v>7.1338649999999992</v>
+        <f t="shared" ref="E180:G180" si="9">E258+E259</f>
+        <v>3.8967000000000002E-2</v>
       </c>
       <c r="F180" s="216">
-        <f>28*F258+265*F259</f>
-        <v>6.6657679999999999</v>
+        <f t="shared" si="9"/>
+        <v>3.6409999999999998E-2</v>
       </c>
       <c r="G180" s="216">
-        <f>28*G258+265*G259</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H180" s="78"/>
@@ -13254,10 +13296,10 @@
       <c r="I207" s="97"/>
     </row>
     <row r="208" spans="1:12">
-      <c r="A208" s="234" t="s">
+      <c r="A208" s="236" t="s">
         <v>623</v>
       </c>
-      <c r="B208" s="226"/>
+      <c r="B208" s="228"/>
       <c r="C208" s="103"/>
       <c r="D208" s="103"/>
       <c r="E208" s="103"/>
@@ -13267,10 +13309,10 @@
       <c r="I208" s="103"/>
     </row>
     <row r="209" spans="1:10">
-      <c r="A209" s="230" t="s">
+      <c r="A209" s="232" t="s">
         <v>822</v>
       </c>
-      <c r="B209" s="226"/>
+      <c r="B209" s="228"/>
       <c r="C209" s="103"/>
       <c r="D209" s="103"/>
       <c r="E209" s="103"/>
@@ -13280,10 +13322,10 @@
       <c r="I209" s="103"/>
     </row>
     <row r="210" spans="1:10">
-      <c r="A210" s="230" t="s">
+      <c r="A210" s="232" t="s">
         <v>823</v>
       </c>
-      <c r="B210" s="226"/>
+      <c r="B210" s="228"/>
       <c r="C210" s="103"/>
       <c r="D210" s="103"/>
       <c r="E210" s="103"/>
@@ -13293,10 +13335,10 @@
       <c r="I210" s="103"/>
     </row>
     <row r="211" spans="1:10">
-      <c r="A211" s="230" t="s">
+      <c r="A211" s="232" t="s">
         <v>824</v>
       </c>
-      <c r="B211" s="226"/>
+      <c r="B211" s="228"/>
       <c r="C211" s="103"/>
       <c r="D211" s="103"/>
       <c r="E211" s="103"/>
@@ -13306,10 +13348,10 @@
       <c r="I211" s="103"/>
     </row>
     <row r="212" spans="1:10">
-      <c r="A212" s="230" t="s">
+      <c r="A212" s="232" t="s">
         <v>631</v>
       </c>
-      <c r="B212" s="226"/>
+      <c r="B212" s="228"/>
       <c r="C212" s="103"/>
       <c r="D212" s="103"/>
       <c r="E212" s="103"/>
@@ -13319,10 +13361,10 @@
       <c r="I212" s="103"/>
     </row>
     <row r="213" spans="1:10">
-      <c r="A213" s="230" t="s">
+      <c r="A213" s="232" t="s">
         <v>632</v>
       </c>
-      <c r="B213" s="226"/>
+      <c r="B213" s="228"/>
       <c r="C213" s="103"/>
       <c r="D213" s="103"/>
       <c r="E213" s="103"/>
@@ -13332,10 +13374,10 @@
       <c r="I213" s="103"/>
     </row>
     <row r="214" spans="1:10">
-      <c r="A214" s="230" t="s">
+      <c r="A214" s="232" t="s">
         <v>633</v>
       </c>
-      <c r="B214" s="226"/>
+      <c r="B214" s="228"/>
       <c r="C214" s="103"/>
       <c r="D214" s="103"/>
       <c r="E214" s="103"/>
@@ -13345,10 +13387,10 @@
       <c r="I214" s="103"/>
     </row>
     <row r="215" spans="1:10">
-      <c r="A215" s="230" t="s">
+      <c r="A215" s="232" t="s">
         <v>825</v>
       </c>
-      <c r="B215" s="226"/>
+      <c r="B215" s="228"/>
       <c r="C215" s="103"/>
       <c r="D215" s="103"/>
       <c r="E215" s="103"/>
@@ -13358,10 +13400,10 @@
       <c r="I215" s="103"/>
     </row>
     <row r="216" spans="1:10">
-      <c r="A216" s="230" t="s">
+      <c r="A216" s="232" t="s">
         <v>826</v>
       </c>
-      <c r="B216" s="226"/>
+      <c r="B216" s="228"/>
       <c r="C216" s="103"/>
       <c r="D216" s="103"/>
       <c r="E216" s="103"/>
@@ -13371,8 +13413,8 @@
       <c r="I216" s="103"/>
     </row>
     <row r="217" spans="1:10">
-      <c r="A217" s="230"/>
-      <c r="B217" s="226"/>
+      <c r="A217" s="232"/>
+      <c r="B217" s="228"/>
       <c r="C217" s="103"/>
       <c r="D217" s="103"/>
       <c r="E217" s="103"/>
@@ -13402,32 +13444,32 @@
       <c r="I219" s="97"/>
     </row>
     <row r="220" spans="1:10">
-      <c r="A220" s="233" t="s">
+      <c r="A220" s="235" t="s">
         <v>827</v>
       </c>
-      <c r="B220" s="218"/>
-      <c r="C220" s="218"/>
-      <c r="D220" s="218"/>
-      <c r="E220" s="218"/>
-      <c r="F220" s="218"/>
-      <c r="G220" s="218"/>
-      <c r="H220" s="218"/>
-      <c r="I220" s="218"/>
-      <c r="J220" s="218"/>
+      <c r="B220" s="220"/>
+      <c r="C220" s="220"/>
+      <c r="D220" s="220"/>
+      <c r="E220" s="220"/>
+      <c r="F220" s="220"/>
+      <c r="G220" s="220"/>
+      <c r="H220" s="220"/>
+      <c r="I220" s="220"/>
+      <c r="J220" s="220"/>
     </row>
     <row r="221" spans="1:10">
-      <c r="A221" s="232" t="s">
+      <c r="A221" s="234" t="s">
         <v>828</v>
       </c>
-      <c r="B221" s="218"/>
-      <c r="C221" s="218"/>
-      <c r="D221" s="218"/>
-      <c r="E221" s="218"/>
-      <c r="F221" s="218"/>
-      <c r="G221" s="218"/>
-      <c r="H221" s="218"/>
-      <c r="I221" s="218"/>
-      <c r="J221" s="218"/>
+      <c r="B221" s="220"/>
+      <c r="C221" s="220"/>
+      <c r="D221" s="220"/>
+      <c r="E221" s="220"/>
+      <c r="F221" s="220"/>
+      <c r="G221" s="220"/>
+      <c r="H221" s="220"/>
+      <c r="I221" s="220"/>
+      <c r="J221" s="220"/>
     </row>
     <row r="222" spans="1:10">
       <c r="A222" s="164"/>
@@ -13442,32 +13484,32 @@
       <c r="J222" s="104"/>
     </row>
     <row r="223" spans="1:10">
-      <c r="A223" s="233" t="s">
+      <c r="A223" s="235" t="s">
         <v>829</v>
       </c>
-      <c r="B223" s="218"/>
-      <c r="C223" s="218"/>
-      <c r="D223" s="218"/>
-      <c r="E223" s="218"/>
-      <c r="F223" s="218"/>
-      <c r="G223" s="218"/>
-      <c r="H223" s="218"/>
-      <c r="I223" s="218"/>
-      <c r="J223" s="218"/>
+      <c r="B223" s="220"/>
+      <c r="C223" s="220"/>
+      <c r="D223" s="220"/>
+      <c r="E223" s="220"/>
+      <c r="F223" s="220"/>
+      <c r="G223" s="220"/>
+      <c r="H223" s="220"/>
+      <c r="I223" s="220"/>
+      <c r="J223" s="220"/>
     </row>
     <row r="224" spans="1:10">
-      <c r="A224" s="232" t="s">
+      <c r="A224" s="234" t="s">
         <v>830</v>
       </c>
-      <c r="B224" s="218"/>
-      <c r="C224" s="218"/>
-      <c r="D224" s="218"/>
-      <c r="E224" s="218"/>
-      <c r="F224" s="218"/>
-      <c r="G224" s="218"/>
-      <c r="H224" s="218"/>
-      <c r="I224" s="218"/>
-      <c r="J224" s="218"/>
+      <c r="B224" s="220"/>
+      <c r="C224" s="220"/>
+      <c r="D224" s="220"/>
+      <c r="E224" s="220"/>
+      <c r="F224" s="220"/>
+      <c r="G224" s="220"/>
+      <c r="H224" s="220"/>
+      <c r="I224" s="220"/>
+      <c r="J224" s="220"/>
     </row>
     <row r="225" spans="1:10">
       <c r="A225" s="164"/>
@@ -13482,32 +13524,32 @@
       <c r="J225" s="104"/>
     </row>
     <row r="226" spans="1:10">
-      <c r="A226" s="233" t="s">
+      <c r="A226" s="235" t="s">
         <v>831</v>
       </c>
-      <c r="B226" s="218"/>
-      <c r="C226" s="218"/>
-      <c r="D226" s="218"/>
-      <c r="E226" s="218"/>
-      <c r="F226" s="218"/>
-      <c r="G226" s="218"/>
-      <c r="H226" s="218"/>
-      <c r="I226" s="218"/>
-      <c r="J226" s="218"/>
+      <c r="B226" s="220"/>
+      <c r="C226" s="220"/>
+      <c r="D226" s="220"/>
+      <c r="E226" s="220"/>
+      <c r="F226" s="220"/>
+      <c r="G226" s="220"/>
+      <c r="H226" s="220"/>
+      <c r="I226" s="220"/>
+      <c r="J226" s="220"/>
     </row>
     <row r="227" spans="1:10">
-      <c r="A227" s="232" t="s">
+      <c r="A227" s="234" t="s">
         <v>832</v>
       </c>
-      <c r="B227" s="218"/>
-      <c r="C227" s="218"/>
-      <c r="D227" s="218"/>
-      <c r="E227" s="218"/>
-      <c r="F227" s="218"/>
-      <c r="G227" s="218"/>
-      <c r="H227" s="218"/>
-      <c r="I227" s="218"/>
-      <c r="J227" s="218"/>
+      <c r="B227" s="220"/>
+      <c r="C227" s="220"/>
+      <c r="D227" s="220"/>
+      <c r="E227" s="220"/>
+      <c r="F227" s="220"/>
+      <c r="G227" s="220"/>
+      <c r="H227" s="220"/>
+      <c r="I227" s="220"/>
+      <c r="J227" s="220"/>
     </row>
     <row r="228" spans="1:10">
       <c r="B228" s="97"/>
@@ -13520,32 +13562,32 @@
       <c r="I228" s="97"/>
     </row>
     <row r="229" spans="1:10">
-      <c r="A229" s="233" t="s">
+      <c r="A229" s="235" t="s">
         <v>833</v>
       </c>
-      <c r="B229" s="218"/>
-      <c r="C229" s="218"/>
-      <c r="D229" s="218"/>
-      <c r="E229" s="218"/>
-      <c r="F229" s="218"/>
-      <c r="G229" s="218"/>
-      <c r="H229" s="218"/>
-      <c r="I229" s="218"/>
-      <c r="J229" s="218"/>
+      <c r="B229" s="220"/>
+      <c r="C229" s="220"/>
+      <c r="D229" s="220"/>
+      <c r="E229" s="220"/>
+      <c r="F229" s="220"/>
+      <c r="G229" s="220"/>
+      <c r="H229" s="220"/>
+      <c r="I229" s="220"/>
+      <c r="J229" s="220"/>
     </row>
     <row r="230" spans="1:10">
-      <c r="A230" s="232" t="s">
+      <c r="A230" s="234" t="s">
         <v>834</v>
       </c>
-      <c r="B230" s="218"/>
-      <c r="C230" s="218"/>
-      <c r="D230" s="218"/>
-      <c r="E230" s="218"/>
-      <c r="F230" s="218"/>
-      <c r="G230" s="218"/>
-      <c r="H230" s="218"/>
-      <c r="I230" s="218"/>
-      <c r="J230" s="218"/>
+      <c r="B230" s="220"/>
+      <c r="C230" s="220"/>
+      <c r="D230" s="220"/>
+      <c r="E230" s="220"/>
+      <c r="F230" s="220"/>
+      <c r="G230" s="220"/>
+      <c r="H230" s="220"/>
+      <c r="I230" s="220"/>
+      <c r="J230" s="220"/>
     </row>
     <row r="231" spans="1:10">
       <c r="B231" s="97"/>
@@ -13558,32 +13600,32 @@
       <c r="I231" s="97"/>
     </row>
     <row r="232" spans="1:10">
-      <c r="A232" s="233" t="s">
+      <c r="A232" s="235" t="s">
         <v>636</v>
       </c>
-      <c r="B232" s="218"/>
-      <c r="C232" s="218"/>
-      <c r="D232" s="218"/>
-      <c r="E232" s="218"/>
-      <c r="F232" s="218"/>
-      <c r="G232" s="218"/>
-      <c r="H232" s="218"/>
-      <c r="I232" s="218"/>
-      <c r="J232" s="218"/>
+      <c r="B232" s="220"/>
+      <c r="C232" s="220"/>
+      <c r="D232" s="220"/>
+      <c r="E232" s="220"/>
+      <c r="F232" s="220"/>
+      <c r="G232" s="220"/>
+      <c r="H232" s="220"/>
+      <c r="I232" s="220"/>
+      <c r="J232" s="220"/>
     </row>
     <row r="233" spans="1:10">
-      <c r="A233" s="232" t="s">
+      <c r="A233" s="234" t="s">
         <v>835</v>
       </c>
-      <c r="B233" s="218"/>
-      <c r="C233" s="218"/>
-      <c r="D233" s="218"/>
-      <c r="E233" s="218"/>
-      <c r="F233" s="218"/>
-      <c r="G233" s="218"/>
-      <c r="H233" s="218"/>
-      <c r="I233" s="218"/>
-      <c r="J233" s="218"/>
+      <c r="B233" s="220"/>
+      <c r="C233" s="220"/>
+      <c r="D233" s="220"/>
+      <c r="E233" s="220"/>
+      <c r="F233" s="220"/>
+      <c r="G233" s="220"/>
+      <c r="H233" s="220"/>
+      <c r="I233" s="220"/>
+      <c r="J233" s="220"/>
     </row>
     <row r="234" spans="1:10">
       <c r="B234" s="97"/>
@@ -13672,7 +13714,7 @@
       <c r="H240" s="100"/>
       <c r="I240" s="100"/>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:11">
       <c r="A241" s="22" t="s">
         <v>840</v>
       </c>
@@ -13687,7 +13729,7 @@
       <c r="H241" s="100"/>
       <c r="I241" s="100"/>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:11">
       <c r="A242" s="22" t="s">
         <v>841</v>
       </c>
@@ -13702,7 +13744,7 @@
       <c r="H242" s="100"/>
       <c r="I242" s="100"/>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:11">
       <c r="A243" s="22" t="s">
         <v>842</v>
       </c>
@@ -13717,7 +13759,7 @@
       <c r="H243" s="101"/>
       <c r="I243" s="101"/>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:11">
       <c r="A244" s="22" t="s">
         <v>843</v>
       </c>
@@ -13732,7 +13774,7 @@
       <c r="H244" s="101"/>
       <c r="I244" s="101"/>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:11">
       <c r="A245" s="22" t="s">
         <v>844</v>
       </c>
@@ -13747,7 +13789,7 @@
       <c r="H245" s="101"/>
       <c r="I245" s="101"/>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:11">
       <c r="A246" s="22" t="s">
         <v>841</v>
       </c>
@@ -13762,12 +13804,12 @@
       <c r="H246" s="101"/>
       <c r="I246" s="101"/>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:11">
       <c r="A250" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:11">
       <c r="A251" s="22" t="s">
         <v>659</v>
       </c>
@@ -13778,16 +13820,16 @@
         <v>192.02484769803729</v>
       </c>
       <c r="E251">
-        <v>218.0500809836573</v>
+        <v>221.19946624142241</v>
       </c>
       <c r="F251">
-        <v>286.12329886576202</v>
+        <v>291.60473799632678</v>
       </c>
       <c r="G251">
-        <v>378.26073777409113</v>
-      </c>
-    </row>
-    <row r="252" spans="1:9">
+        <v>387.50337752980528</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11">
       <c r="A252" t="s">
         <v>846</v>
       </c>
@@ -13799,19 +13841,19 @@
         <v>1.8276473667706143</v>
       </c>
       <c r="E252">
-        <f t="shared" ref="E252:G252" si="9">E23/E251</f>
-        <v>1.5389560823992434</v>
+        <f>E23/E251</f>
+        <v>1.7949769533336146</v>
       </c>
       <c r="F252">
-        <f t="shared" si="9"/>
-        <v>1.4690597028594603</v>
+        <f>F23/F251</f>
+        <v>1.8083867908658213</v>
       </c>
       <c r="G252">
-        <f t="shared" si="9"/>
-        <v>1.3909377218957639</v>
-      </c>
-    </row>
-    <row r="253" spans="1:9">
+        <f>G23/G251</f>
+        <v>1.8130416495307522</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11">
       <c r="A253" t="s">
         <v>847</v>
       </c>
@@ -13822,16 +13864,16 @@
         <v>3113.4730612226449</v>
       </c>
       <c r="E253">
-        <v>3674.200283951865</v>
+        <v>3708.4644596254252</v>
       </c>
       <c r="F253">
-        <v>3743.2139728916668</v>
+        <v>3837.2995593855539</v>
       </c>
       <c r="G253">
-        <v>6066.614513002045</v>
-      </c>
-    </row>
-    <row r="254" spans="1:9">
+        <v>6229.0165570380477</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11">
       <c r="A254" t="s">
         <v>849</v>
       </c>
@@ -13851,7 +13893,7 @@
         <v>0.78998940677966101</v>
       </c>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:11">
       <c r="A255" t="s">
         <v>850</v>
       </c>
@@ -13871,7 +13913,7 @@
         <v>0.21001059322033899</v>
       </c>
     </row>
-    <row r="256" spans="1:9">
+    <row r="256" spans="1:11">
       <c r="A256" t="s">
         <v>851</v>
       </c>
@@ -13886,6 +13928,14 @@
       </c>
       <c r="F256">
         <v>3.3069000000000001E-2</v>
+      </c>
+      <c r="J256">
+        <f>1256/1000</f>
+        <v>1.256</v>
+      </c>
+      <c r="K256">
+        <f>J256/28</f>
+        <v>4.4857142857142859E-2</v>
       </c>
     </row>
     <row r="257" spans="1:6">
@@ -14019,22 +14069,22 @@
       <c r="E3" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="64.5" customHeight="1">
-      <c r="A5" s="237" t="s">
+      <c r="A5" s="239" t="s">
         <v>857</v>
       </c>
-      <c r="B5" s="225"/>
-      <c r="C5" s="225"/>
-      <c r="D5" s="225"/>
-      <c r="E5" s="226"/>
+      <c r="B5" s="227"/>
+      <c r="C5" s="227"/>
+      <c r="D5" s="227"/>
+      <c r="E5" s="228"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A7" s="235" t="s">
+      <c r="A7" s="237" t="s">
         <v>858</v>
       </c>
-      <c r="B7" s="236"/>
-      <c r="C7" s="236"/>
-      <c r="D7" s="236"/>
-      <c r="E7" s="236"/>
+      <c r="B7" s="238"/>
+      <c r="C7" s="238"/>
+      <c r="D7" s="238"/>
+      <c r="E7" s="238"/>
     </row>
     <row r="8" spans="1:5" ht="47.25" customHeight="1">
       <c r="A8" s="47" t="s">
@@ -14115,13 +14165,13 @@
       <c r="D14" s="167"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A15" s="235" t="s">
+      <c r="A15" s="237" t="s">
         <v>871</v>
       </c>
-      <c r="B15" s="236"/>
-      <c r="C15" s="236"/>
-      <c r="D15" s="236"/>
-      <c r="E15" s="236"/>
+      <c r="B15" s="238"/>
+      <c r="C15" s="238"/>
+      <c r="D15" s="238"/>
+      <c r="E15" s="238"/>
     </row>
     <row r="16" spans="1:5" ht="47.25" customHeight="1">
       <c r="A16" s="47" t="s">
@@ -14203,13 +14253,13 @@
       <c r="D22" s="167"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A23" s="235" t="s">
+      <c r="A23" s="237" t="s">
         <v>879</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
-      <c r="D23" s="236"/>
-      <c r="E23" s="236"/>
+      <c r="B23" s="238"/>
+      <c r="C23" s="238"/>
+      <c r="D23" s="238"/>
+      <c r="E23" s="238"/>
     </row>
     <row r="24" spans="1:6" ht="47.25" customHeight="1">
       <c r="A24" s="47" t="s">
@@ -14290,13 +14340,13 @@
       <c r="D30" s="167"/>
     </row>
     <row r="31" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A31" s="235" t="s">
+      <c r="A31" s="237" t="s">
         <v>885</v>
       </c>
-      <c r="B31" s="236"/>
-      <c r="C31" s="236"/>
-      <c r="D31" s="236"/>
-      <c r="E31" s="236"/>
+      <c r="B31" s="238"/>
+      <c r="C31" s="238"/>
+      <c r="D31" s="238"/>
+      <c r="E31" s="238"/>
     </row>
     <row r="32" spans="1:6" ht="47.25" customHeight="1">
       <c r="A32" s="47" t="s">
@@ -14377,13 +14427,13 @@
       <c r="D38" s="167"/>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A39" s="235" t="s">
+      <c r="A39" s="237" t="s">
         <v>888</v>
       </c>
-      <c r="B39" s="236"/>
-      <c r="C39" s="236"/>
-      <c r="D39" s="236"/>
-      <c r="E39" s="236"/>
+      <c r="B39" s="238"/>
+      <c r="C39" s="238"/>
+      <c r="D39" s="238"/>
+      <c r="E39" s="238"/>
     </row>
     <row r="40" spans="1:5" ht="47.25" customHeight="1">
       <c r="A40" s="47" t="s">
@@ -21682,13 +21732,13 @@
       <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" ht="64.5" customHeight="1">
-      <c r="A5" s="237" t="s">
+      <c r="A5" s="239" t="s">
         <v>973</v>
       </c>
-      <c r="B5" s="225"/>
-      <c r="C5" s="225"/>
-      <c r="D5" s="225"/>
-      <c r="E5" s="226"/>
+      <c r="B5" s="227"/>
+      <c r="C5" s="227"/>
+      <c r="D5" s="227"/>
+      <c r="E5" s="228"/>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="B6" s="46"/>
@@ -65927,10 +65977,10 @@
       <c r="J317" s="69"/>
     </row>
     <row r="318" spans="1:12">
-      <c r="A318" s="231" t="s">
+      <c r="A318" s="233" t="s">
         <v>623</v>
       </c>
-      <c r="B318" s="226"/>
+      <c r="B318" s="228"/>
       <c r="C318" s="89"/>
       <c r="D318" s="89"/>
       <c r="E318" s="89"/>
@@ -65941,10 +65991,10 @@
       <c r="J318" s="69"/>
     </row>
     <row r="319" spans="1:12">
-      <c r="A319" s="230" t="s">
+      <c r="A319" s="232" t="s">
         <v>624</v>
       </c>
-      <c r="B319" s="226"/>
+      <c r="B319" s="228"/>
       <c r="C319" s="89"/>
       <c r="D319" s="89"/>
       <c r="E319" s="89"/>
@@ -65955,10 +66005,10 @@
       <c r="J319" s="69"/>
     </row>
     <row r="320" spans="1:12">
-      <c r="A320" s="230" t="s">
+      <c r="A320" s="232" t="s">
         <v>625</v>
       </c>
-      <c r="B320" s="226"/>
+      <c r="B320" s="228"/>
       <c r="C320" s="89"/>
       <c r="D320" s="89"/>
       <c r="E320" s="89"/>
@@ -65969,10 +66019,10 @@
       <c r="J320" s="69"/>
     </row>
     <row r="321" spans="1:10">
-      <c r="A321" s="230" t="s">
+      <c r="A321" s="232" t="s">
         <v>626</v>
       </c>
-      <c r="B321" s="226"/>
+      <c r="B321" s="228"/>
       <c r="C321" s="89"/>
       <c r="D321" s="89"/>
       <c r="E321" s="89"/>
@@ -65983,10 +66033,10 @@
       <c r="J321" s="69"/>
     </row>
     <row r="322" spans="1:10">
-      <c r="A322" s="230" t="s">
+      <c r="A322" s="232" t="s">
         <v>627</v>
       </c>
-      <c r="B322" s="226"/>
+      <c r="B322" s="228"/>
       <c r="C322" s="89"/>
       <c r="D322" s="89"/>
       <c r="E322" s="89"/>
@@ -65997,10 +66047,10 @@
       <c r="J322" s="69"/>
     </row>
     <row r="323" spans="1:10">
-      <c r="A323" s="230" t="s">
+      <c r="A323" s="232" t="s">
         <v>628</v>
       </c>
-      <c r="B323" s="226"/>
+      <c r="B323" s="228"/>
       <c r="C323" s="89"/>
       <c r="D323" s="89"/>
       <c r="E323" s="89"/>
@@ -66011,10 +66061,10 @@
       <c r="J323" s="69"/>
     </row>
     <row r="324" spans="1:10">
-      <c r="A324" s="230" t="s">
+      <c r="A324" s="232" t="s">
         <v>629</v>
       </c>
-      <c r="B324" s="226"/>
+      <c r="B324" s="228"/>
       <c r="C324" s="89"/>
       <c r="D324" s="89"/>
       <c r="E324" s="89"/>
@@ -66025,10 +66075,10 @@
       <c r="J324" s="69"/>
     </row>
     <row r="325" spans="1:10">
-      <c r="A325" s="230" t="s">
+      <c r="A325" s="232" t="s">
         <v>630</v>
       </c>
-      <c r="B325" s="226"/>
+      <c r="B325" s="228"/>
       <c r="C325" s="89"/>
       <c r="D325" s="89"/>
       <c r="E325" s="89"/>
@@ -66039,10 +66089,10 @@
       <c r="J325" s="69"/>
     </row>
     <row r="326" spans="1:10">
-      <c r="A326" s="230" t="s">
+      <c r="A326" s="232" t="s">
         <v>631</v>
       </c>
-      <c r="B326" s="226"/>
+      <c r="B326" s="228"/>
       <c r="C326" s="89"/>
       <c r="D326" s="89"/>
       <c r="E326" s="89"/>
@@ -66053,10 +66103,10 @@
       <c r="J326" s="69"/>
     </row>
     <row r="327" spans="1:10">
-      <c r="A327" s="230" t="s">
+      <c r="A327" s="232" t="s">
         <v>632</v>
       </c>
-      <c r="B327" s="226"/>
+      <c r="B327" s="228"/>
       <c r="C327" s="89"/>
       <c r="D327" s="89"/>
       <c r="E327" s="89"/>
@@ -66067,10 +66117,10 @@
       <c r="J327" s="69"/>
     </row>
     <row r="328" spans="1:10">
-      <c r="A328" s="230" t="s">
+      <c r="A328" s="232" t="s">
         <v>633</v>
       </c>
-      <c r="B328" s="226"/>
+      <c r="B328" s="228"/>
       <c r="C328" s="89"/>
       <c r="D328" s="89"/>
       <c r="E328" s="89"/>
@@ -66081,10 +66131,10 @@
       <c r="J328" s="69"/>
     </row>
     <row r="329" spans="1:10">
-      <c r="A329" s="230" t="s">
+      <c r="A329" s="232" t="s">
         <v>634</v>
       </c>
-      <c r="B329" s="226"/>
+      <c r="B329" s="228"/>
       <c r="C329" s="89"/>
       <c r="D329" s="89"/>
       <c r="E329" s="89"/>
@@ -66095,10 +66145,10 @@
       <c r="J329" s="69"/>
     </row>
     <row r="330" spans="1:10">
-      <c r="A330" s="230" t="s">
+      <c r="A330" s="232" t="s">
         <v>635</v>
       </c>
-      <c r="B330" s="226"/>
+      <c r="B330" s="228"/>
       <c r="C330" s="89"/>
       <c r="D330" s="89"/>
       <c r="E330" s="89"/>
@@ -66133,32 +66183,32 @@
       <c r="J332" s="69"/>
     </row>
     <row r="333" spans="1:10">
-      <c r="A333" s="233" t="s">
+      <c r="A333" s="235" t="s">
         <v>636</v>
       </c>
-      <c r="B333" s="218"/>
-      <c r="C333" s="218"/>
-      <c r="D333" s="218"/>
-      <c r="E333" s="218"/>
-      <c r="F333" s="218"/>
-      <c r="G333" s="218"/>
-      <c r="H333" s="218"/>
-      <c r="I333" s="218"/>
-      <c r="J333" s="218"/>
+      <c r="B333" s="220"/>
+      <c r="C333" s="220"/>
+      <c r="D333" s="220"/>
+      <c r="E333" s="220"/>
+      <c r="F333" s="220"/>
+      <c r="G333" s="220"/>
+      <c r="H333" s="220"/>
+      <c r="I333" s="220"/>
+      <c r="J333" s="220"/>
     </row>
     <row r="334" spans="1:10" ht="33.75" customHeight="1">
-      <c r="A334" s="232" t="s">
+      <c r="A334" s="234" t="s">
         <v>637</v>
       </c>
-      <c r="B334" s="218"/>
-      <c r="C334" s="218"/>
-      <c r="D334" s="218"/>
-      <c r="E334" s="218"/>
-      <c r="F334" s="218"/>
-      <c r="G334" s="218"/>
-      <c r="H334" s="218"/>
-      <c r="I334" s="218"/>
-      <c r="J334" s="218"/>
+      <c r="B334" s="220"/>
+      <c r="C334" s="220"/>
+      <c r="D334" s="220"/>
+      <c r="E334" s="220"/>
+      <c r="F334" s="220"/>
+      <c r="G334" s="220"/>
+      <c r="H334" s="220"/>
+      <c r="I334" s="220"/>
+      <c r="J334" s="220"/>
     </row>
     <row r="335" spans="1:10">
       <c r="A335" s="88"/>

</xml_diff>

<commit_message>
Corrected and ran pwr sector, mostly working except for autogen twh
</commit_message>
<xml_diff>
--- a/input/WB1.xlsx
+++ b/input/WB1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DDPTemplateAutomationV2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91FFB18-F451-4AFB-9612-FA71FCD58D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE98A4C-A824-41F2-87D1-8A8D7D64E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="888" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="888" firstSheet="12" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User guide" sheetId="1" r:id="rId1"/>
@@ -9095,7 +9095,7 @@
   </sheetPr>
   <dimension ref="A1:L259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D179" sqref="D179:G180"/>
     </sheetView>
   </sheetViews>
@@ -12782,15 +12782,15 @@
         <v>0.10173</v>
       </c>
       <c r="E179" s="216">
-        <f t="shared" ref="E179:G179" si="8">E256+E257</f>
+        <f>E256+E257</f>
         <v>9.7095000000000001E-2</v>
       </c>
       <c r="F179" s="216">
-        <f t="shared" si="8"/>
+        <f>F256+F257</f>
         <v>9.5662999999999998E-2</v>
       </c>
       <c r="G179" s="216">
-        <f t="shared" si="8"/>
+        <f>G256+G257</f>
         <v>0</v>
       </c>
       <c r="H179" s="78"/>
@@ -12812,15 +12812,15 @@
         <v>4.9299000000000003E-2</v>
       </c>
       <c r="E180" s="216">
-        <f t="shared" ref="E180:G180" si="9">E258+E259</f>
+        <f>E258+E259</f>
         <v>3.8967000000000002E-2</v>
       </c>
       <c r="F180" s="216">
-        <f t="shared" si="9"/>
+        <f>F258+F259</f>
         <v>3.6409999999999998E-2</v>
       </c>
       <c r="G180" s="216">
-        <f t="shared" si="9"/>
+        <f>G258+G259</f>
         <v>0</v>
       </c>
       <c r="H180" s="78"/>
@@ -37091,10 +37091,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:L165"/>
+  <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="D27:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -37231,19 +37231,19 @@
       </c>
       <c r="D7" s="172">
         <f t="shared" si="1"/>
-        <v>912.04324872474263</v>
+        <v>926.47334960024193</v>
       </c>
       <c r="E7" s="172">
         <f t="shared" si="1"/>
-        <v>636.54306800663358</v>
+        <v>604.13474807231455</v>
       </c>
       <c r="F7" s="172">
         <f t="shared" si="1"/>
-        <v>337.54694338972325</v>
+        <v>60.208162885254403</v>
       </c>
       <c r="G7" s="172">
         <f t="shared" si="1"/>
-        <v>193.64297609661989</v>
+        <v>0.5744964592361026</v>
       </c>
       <c r="H7" s="172" t="e">
         <f t="shared" si="1"/>
@@ -37267,19 +37267,19 @@
       </c>
       <c r="D8" s="172">
         <f t="shared" si="2"/>
-        <v>222.92578700000001</v>
+        <v>205.88177100000004</v>
       </c>
       <c r="E8" s="172">
         <f t="shared" si="2"/>
-        <v>257.50246800000002</v>
+        <v>219.21848300000002</v>
       </c>
       <c r="F8" s="172">
         <f t="shared" si="2"/>
-        <v>360.93713300000002</v>
+        <v>277.89987600000001</v>
       </c>
       <c r="G8" s="172">
         <f t="shared" si="2"/>
-        <v>482.12010000000004</v>
+        <v>573.32642299999998</v>
       </c>
       <c r="H8" s="172">
         <f t="shared" si="2"/>
@@ -37303,19 +37303,19 @@
       </c>
       <c r="D9" s="172">
         <f t="shared" si="3"/>
-        <v>203.317959</v>
+        <v>190.74397399999998</v>
       </c>
       <c r="E9" s="172">
         <f t="shared" si="3"/>
-        <v>163.91141099999999</v>
+        <v>132.43750299999999</v>
       </c>
       <c r="F9" s="172">
         <f t="shared" si="3"/>
-        <v>121.83322600000001</v>
+        <v>16.731840999999999</v>
       </c>
       <c r="G9" s="172">
         <f t="shared" si="3"/>
-        <v>93.359171000000003</v>
+        <v>0.329374</v>
       </c>
       <c r="H9" s="172">
         <f t="shared" si="3"/>
@@ -37339,19 +37339,19 @@
       </c>
       <c r="D10" s="172">
         <f t="shared" si="4"/>
-        <v>0.85809299999999999</v>
+        <v>0.80529499999999998</v>
       </c>
       <c r="E10" s="172">
         <f t="shared" si="4"/>
-        <v>0.67531600000000003</v>
+        <v>0.54780899999999999</v>
       </c>
       <c r="F10" s="172">
         <f t="shared" si="4"/>
-        <v>0.47049600000000003</v>
+        <v>7.1572999999999998E-2</v>
       </c>
       <c r="G10" s="172">
         <f t="shared" si="4"/>
-        <v>0.198546</v>
+        <v>6.4260000000000003E-3</v>
       </c>
       <c r="H10" s="172">
         <f t="shared" si="4"/>
@@ -37387,7 +37387,7 @@
       </c>
       <c r="G11" s="172">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-2.2426750000000002</v>
       </c>
       <c r="H11" s="172">
         <f t="shared" si="5"/>
@@ -37459,7 +37459,7 @@
       </c>
       <c r="G13" s="172">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-2.2426750000000002</v>
       </c>
       <c r="H13" s="172">
         <f t="shared" si="6"/>
@@ -37764,16 +37764,16 @@
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="44">
-        <v>0.381135</v>
+        <v>0.67584299999999997</v>
       </c>
       <c r="E27" s="44">
-        <v>3.1940900000000001</v>
+        <v>1.6189480000000001</v>
       </c>
       <c r="F27" s="44">
-        <v>18.067983000000002</v>
+        <v>10.799037</v>
       </c>
       <c r="G27" s="44">
-        <v>29.505915999999999</v>
+        <v>27.571095</v>
       </c>
       <c r="H27" s="44"/>
       <c r="I27" s="44"/>
@@ -37792,16 +37792,16 @@
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="44">
-        <v>2.5942590000000001</v>
+        <v>2.8111920000000001</v>
       </c>
       <c r="E28" s="44">
-        <v>7.7600259999999999</v>
+        <v>9.4071079999999991</v>
       </c>
       <c r="F28" s="44">
-        <v>24.878160999999999</v>
+        <v>21.152494000000001</v>
       </c>
       <c r="G28" s="44">
-        <v>36.388005999999997</v>
+        <v>55.583309999999997</v>
       </c>
       <c r="H28" s="44"/>
       <c r="I28" s="44"/>
@@ -37820,16 +37820,16 @@
       </c>
       <c r="C29" s="44"/>
       <c r="D29" s="44">
-        <v>46.795530999999997</v>
+        <v>44.349556999999997</v>
       </c>
       <c r="E29" s="44">
-        <v>49.150874999999999</v>
+        <v>45.183309999999999</v>
       </c>
       <c r="F29" s="44">
-        <v>55.054310999999998</v>
+        <v>48.300584000000001</v>
       </c>
       <c r="G29" s="44">
-        <v>62.058300000000003</v>
+        <v>56.196263999999999</v>
       </c>
       <c r="H29" s="44"/>
       <c r="I29" s="44"/>
@@ -37848,16 +37848,16 @@
       </c>
       <c r="C30" s="44"/>
       <c r="D30" s="44">
-        <v>35.914853000000001</v>
+        <v>38.590715000000003</v>
       </c>
       <c r="E30" s="44">
-        <v>35.410311999999998</v>
+        <v>38.397942</v>
       </c>
       <c r="F30" s="44">
-        <v>33.533729999999998</v>
+        <v>34.688687999999999</v>
       </c>
       <c r="G30" s="44">
-        <v>35.692624000000002</v>
+        <v>43.542957999999999</v>
       </c>
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
@@ -37876,16 +37876,16 @@
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="44">
-        <v>41.116880999999999</v>
+        <v>42.258926000000002</v>
       </c>
       <c r="E31" s="44">
-        <v>47.997081000000001</v>
+        <v>44.030579000000003</v>
       </c>
       <c r="F31" s="44">
-        <v>56.317771</v>
+        <v>54.762407000000003</v>
       </c>
       <c r="G31" s="44">
-        <v>71.486621</v>
+        <v>93.838811000000007</v>
       </c>
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
@@ -37904,16 +37904,16 @@
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="44">
-        <v>43.854495</v>
+        <v>33.195484</v>
       </c>
       <c r="E32" s="44">
-        <v>54.324787999999998</v>
+        <v>37.512763999999997</v>
       </c>
       <c r="F32" s="44">
-        <v>69.734224999999995</v>
+        <v>58.600819000000001</v>
       </c>
       <c r="G32" s="44">
-        <v>114.79220100000001</v>
+        <v>139.90884600000001</v>
       </c>
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
@@ -37932,16 +37932,16 @@
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="44">
-        <v>6.0311589999999997</v>
+        <v>5.4756830000000001</v>
       </c>
       <c r="E33" s="44">
-        <v>8.2170249999999996</v>
+        <v>6.2171760000000003</v>
       </c>
       <c r="F33" s="44">
-        <v>11.97457</v>
+        <v>7.8482050000000001</v>
       </c>
       <c r="G33" s="44">
-        <v>10.695485</v>
+        <v>20.504926000000001</v>
       </c>
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
@@ -37982,16 +37982,16 @@
       </c>
       <c r="C35" s="44"/>
       <c r="D35" s="44">
-        <v>11.049625000000001</v>
+        <v>10.005996</v>
       </c>
       <c r="E35" s="44">
-        <v>10.007019</v>
+        <v>9.8328589999999991</v>
       </c>
       <c r="F35" s="44">
-        <v>26.019756999999998</v>
+        <v>6.7078480000000003</v>
       </c>
       <c r="G35" s="44">
-        <v>41.817841999999999</v>
+        <v>64.063900000000004</v>
       </c>
       <c r="H35" s="44"/>
       <c r="I35" s="44"/>
@@ -38014,19 +38014,19 @@
       </c>
       <c r="D36" s="150">
         <f t="shared" si="7"/>
-        <v>187.73793799999999</v>
+        <v>177.36339600000002</v>
       </c>
       <c r="E36" s="150">
         <f t="shared" si="7"/>
-        <v>216.061216</v>
+        <v>192.20068599999996</v>
       </c>
       <c r="F36" s="150">
         <f t="shared" si="7"/>
-        <v>295.58050800000001</v>
+        <v>242.86008200000003</v>
       </c>
       <c r="G36" s="150">
         <f t="shared" si="7"/>
-        <v>402.43699500000002</v>
+        <v>501.21011000000004</v>
       </c>
       <c r="H36" s="150">
         <f t="shared" si="7"/>
@@ -38115,16 +38115,16 @@
       </c>
       <c r="C41" s="44"/>
       <c r="D41" s="44">
-        <v>192.138755</v>
+        <v>177.6053</v>
       </c>
       <c r="E41" s="44">
-        <v>157.40144000000001</v>
+        <v>125.686538</v>
       </c>
       <c r="F41" s="44">
-        <v>108.55740299999999</v>
+        <v>15.653499</v>
       </c>
       <c r="G41" s="44">
-        <v>35.201895</v>
+        <v>0.29346</v>
       </c>
       <c r="H41" s="44"/>
       <c r="I41" s="44"/>
@@ -38158,16 +38158,16 @@
         <v>217</v>
       </c>
       <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
+      <c r="D43" s="44">
+        <v>0.70290600000000003</v>
+      </c>
       <c r="E43" s="44">
-        <v>5.1410400000000003</v>
+        <v>0.44257099999999999</v>
       </c>
       <c r="F43" s="44">
-        <v>28.282274000000001</v>
-      </c>
-      <c r="G43" s="44">
-        <v>141.67217299999999</v>
-      </c>
+        <v>0.18223500000000001</v>
+      </c>
+      <c r="G43" s="44"/>
       <c r="H43" s="44"/>
       <c r="I43" s="44"/>
       <c r="J43" s="51"/>
@@ -38185,7 +38185,9 @@
       <c r="D44" s="44"/>
       <c r="E44" s="44"/>
       <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
+      <c r="G44" s="44">
+        <v>5.078538</v>
+      </c>
       <c r="H44" s="44"/>
       <c r="I44" s="44"/>
       <c r="J44" s="51"/>
@@ -38201,13 +38203,13 @@
       </c>
       <c r="C45" s="44"/>
       <c r="D45" s="44">
-        <v>0.83448999999999995</v>
+        <v>0.772065</v>
       </c>
       <c r="E45" s="44">
-        <v>0.80820999999999998</v>
+        <v>0.53770099999999998</v>
       </c>
       <c r="F45" s="44">
-        <v>0.62424999999999997</v>
+        <v>0.14565800000000001</v>
       </c>
       <c r="G45" s="44"/>
       <c r="H45" s="44"/>
@@ -38251,7 +38253,9 @@
       <c r="F47" s="44">
         <v>13.774609</v>
       </c>
-      <c r="G47" s="44"/>
+      <c r="G47" s="44">
+        <v>113.559878</v>
+      </c>
       <c r="H47" s="44"/>
       <c r="I47" s="44"/>
       <c r="J47" s="51"/>
@@ -38311,16 +38315,16 @@
       </c>
       <c r="C50" s="44"/>
       <c r="D50" s="44">
-        <v>5.9389390000000004</v>
+        <v>6.0538509999999999</v>
       </c>
       <c r="E50" s="44">
-        <v>24.235824000000001</v>
+        <v>37.395632999999997</v>
       </c>
       <c r="F50" s="44">
-        <v>103.867097</v>
+        <v>146.25880100000001</v>
       </c>
       <c r="G50" s="44">
-        <v>174.55247800000001</v>
+        <v>262.77042499999999</v>
       </c>
       <c r="H50" s="44"/>
       <c r="I50" s="44"/>
@@ -38337,16 +38341,16 @@
       </c>
       <c r="C51" s="44"/>
       <c r="D51" s="44">
-        <v>4.9562169999999997</v>
+        <v>4.4947489999999997</v>
       </c>
       <c r="E51" s="44">
-        <v>43.87444</v>
+        <v>24.595580000000002</v>
       </c>
       <c r="F51" s="44">
-        <v>86.592744999999994</v>
+        <v>80.047955999999999</v>
       </c>
       <c r="G51" s="44">
-        <v>113.964946</v>
+        <v>131.70258999999999</v>
       </c>
       <c r="H51" s="44"/>
       <c r="I51" s="44"/>
@@ -38363,15 +38367,17 @@
       </c>
       <c r="C52" s="44"/>
       <c r="D52" s="44">
-        <v>2.1617229999999998</v>
+        <v>1.841059</v>
       </c>
       <c r="E52" s="44">
-        <v>2.862444</v>
+        <v>16.086704000000001</v>
       </c>
       <c r="F52" s="44">
-        <v>2.4498950000000002</v>
-      </c>
-      <c r="G52" s="44"/>
+        <v>15.859076999999999</v>
+      </c>
+      <c r="G52" s="44">
+        <v>53.265585000000002</v>
+      </c>
       <c r="H52" s="44"/>
       <c r="I52" s="44"/>
       <c r="J52" s="51"/>
@@ -38388,8 +38394,12 @@
       <c r="C53" s="44"/>
       <c r="D53" s="44"/>
       <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
+      <c r="F53" s="44">
+        <v>5.2788940000000002</v>
+      </c>
+      <c r="G53" s="44">
+        <v>5.9568000000000003</v>
+      </c>
       <c r="H53" s="44"/>
       <c r="I53" s="44"/>
       <c r="J53" s="51"/>
@@ -38440,18 +38450,10 @@
         <v>217</v>
       </c>
       <c r="C56" s="44"/>
-      <c r="D56" s="44">
-        <v>2.483822</v>
-      </c>
-      <c r="E56" s="44">
-        <v>8.7053139999999996</v>
-      </c>
-      <c r="F56" s="44">
-        <v>16.089713</v>
-      </c>
-      <c r="G56" s="44">
-        <v>16.029461000000001</v>
-      </c>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
       <c r="H56" s="44"/>
       <c r="I56" s="44"/>
       <c r="J56" s="51"/>
@@ -38471,19 +38473,19 @@
       </c>
       <c r="D57" s="150">
         <f t="shared" si="8"/>
-        <v>222.92578700000001</v>
+        <v>205.88177100000004</v>
       </c>
       <c r="E57" s="150">
         <f t="shared" si="8"/>
-        <v>257.50246800000002</v>
+        <v>219.21848300000002</v>
       </c>
       <c r="F57" s="150">
         <f t="shared" si="8"/>
-        <v>360.93713300000002</v>
+        <v>277.89987600000001</v>
       </c>
       <c r="G57" s="150">
         <f t="shared" si="8"/>
-        <v>482.12010000000004</v>
+        <v>573.32642299999998</v>
       </c>
       <c r="H57" s="150">
         <f t="shared" si="8"/>
@@ -38556,16 +38558,16 @@
       </c>
       <c r="C61" s="44"/>
       <c r="D61" s="44">
-        <v>202.612459</v>
+        <v>189.77618899999999</v>
       </c>
       <c r="E61" s="44">
-        <v>161.09214499999999</v>
+        <v>131.78553199999999</v>
       </c>
       <c r="F61" s="44">
-        <v>109.48053400000001</v>
+        <v>16.525970000000001</v>
       </c>
       <c r="G61" s="44">
-        <v>33.907575000000001</v>
+        <v>0.329374</v>
       </c>
       <c r="H61" s="44"/>
       <c r="I61" s="44"/>
@@ -38599,16 +38601,16 @@
         <v>1349</v>
       </c>
       <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
+      <c r="D63" s="44">
+        <v>0.31546400000000002</v>
+      </c>
       <c r="E63" s="44">
-        <v>2.1354799999999998</v>
+        <v>0.198626</v>
       </c>
       <c r="F63" s="44">
-        <v>11.820902999999999</v>
-      </c>
-      <c r="G63" s="44">
-        <v>59.451596000000002</v>
-      </c>
+        <v>8.1786999999999999E-2</v>
+      </c>
+      <c r="G63" s="44"/>
       <c r="H63" s="44"/>
       <c r="I63" s="44"/>
       <c r="J63" s="51"/>
@@ -38642,13 +38644,13 @@
       </c>
       <c r="C65" s="44"/>
       <c r="D65" s="44">
-        <v>0.70550000000000002</v>
+        <v>0.65232100000000004</v>
       </c>
       <c r="E65" s="44">
-        <v>0.683786</v>
+        <v>0.453345</v>
       </c>
       <c r="F65" s="44">
-        <v>0.53178899999999996</v>
+        <v>0.124084</v>
       </c>
       <c r="G65" s="44"/>
       <c r="H65" s="44"/>
@@ -38868,19 +38870,19 @@
       </c>
       <c r="D77" s="150">
         <f t="shared" si="9"/>
-        <v>203.317959</v>
+        <v>190.74397399999998</v>
       </c>
       <c r="E77" s="150">
         <f t="shared" si="9"/>
-        <v>163.91141099999999</v>
+        <v>132.43750299999999</v>
       </c>
       <c r="F77" s="150">
         <f t="shared" si="9"/>
-        <v>121.83322600000001</v>
+        <v>16.731840999999999</v>
       </c>
       <c r="G77" s="150">
         <f t="shared" si="9"/>
-        <v>93.359171000000003</v>
+        <v>0.329374</v>
       </c>
       <c r="H77" s="150">
         <f t="shared" si="9"/>
@@ -38919,16 +38921,16 @@
       </c>
       <c r="C79" s="44"/>
       <c r="D79" s="44">
-        <v>0.85809299999999999</v>
+        <v>0.80529499999999998</v>
       </c>
       <c r="E79" s="44">
-        <v>0.67531600000000003</v>
+        <v>0.54780899999999999</v>
       </c>
       <c r="F79" s="44">
-        <v>0.47049600000000003</v>
+        <v>7.1572999999999998E-2</v>
       </c>
       <c r="G79" s="44">
-        <v>0.198546</v>
+        <v>6.4260000000000003E-3</v>
       </c>
       <c r="H79" s="44"/>
       <c r="I79" s="44"/>
@@ -38981,7 +38983,9 @@
       <c r="D82" s="44"/>
       <c r="E82" s="44"/>
       <c r="F82" s="44"/>
-      <c r="G82" s="44"/>
+      <c r="G82" s="44">
+        <v>-2.2426750000000002</v>
+      </c>
       <c r="H82" s="44"/>
       <c r="I82" s="44"/>
       <c r="J82" s="51"/>
@@ -39067,7 +39071,7 @@
       </c>
       <c r="G86" s="150">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-2.2426750000000002</v>
       </c>
       <c r="H86" s="150">
         <f t="shared" si="10"/>
@@ -39110,19 +39114,19 @@
       </c>
       <c r="D88" s="150">
         <f t="shared" si="11"/>
-        <v>204.176052</v>
+        <v>191.54926899999998</v>
       </c>
       <c r="E88" s="150">
         <f t="shared" si="11"/>
-        <v>164.586727</v>
+        <v>132.98531199999999</v>
       </c>
       <c r="F88" s="150">
         <f t="shared" si="11"/>
-        <v>122.30372200000001</v>
+        <v>16.803414</v>
       </c>
       <c r="G88" s="150">
         <f t="shared" si="11"/>
-        <v>93.557716999999997</v>
+        <v>2.5784750000000001</v>
       </c>
       <c r="H88" s="150">
         <f t="shared" si="11"/>
@@ -39177,16 +39181,16 @@
       </c>
       <c r="C91" s="44"/>
       <c r="D91" s="44">
-        <v>39.380000000000003</v>
+        <v>36.064500000000002</v>
       </c>
       <c r="E91" s="44">
-        <v>29.279</v>
+        <v>22.030166999999999</v>
       </c>
       <c r="F91" s="44">
-        <v>17.463999999999999</v>
+        <v>9.4968330000000005</v>
       </c>
       <c r="G91" s="44">
-        <v>5.1950000000000003</v>
+        <v>0.67</v>
       </c>
       <c r="H91" s="44"/>
       <c r="I91" s="44"/>
@@ -39220,16 +39224,16 @@
         <v>1327</v>
       </c>
       <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
+      <c r="D93" s="44">
+        <v>0.15479999999999999</v>
+      </c>
       <c r="E93" s="44">
-        <v>5.8511649999999999</v>
+        <v>9.7466999999999998E-2</v>
       </c>
       <c r="F93" s="44">
-        <v>31.569565000000001</v>
-      </c>
-      <c r="G93" s="44">
-        <v>62.850932999999998</v>
-      </c>
+        <v>4.0133000000000002E-2</v>
+      </c>
+      <c r="G93" s="44"/>
       <c r="H93" s="44"/>
       <c r="I93" s="44"/>
       <c r="J93" s="51"/>
@@ -39247,7 +39251,9 @@
       <c r="D94" s="44"/>
       <c r="E94" s="44"/>
       <c r="F94" s="44"/>
-      <c r="G94" s="44"/>
+      <c r="G94" s="44">
+        <v>11.594836000000001</v>
+      </c>
       <c r="H94" s="44"/>
       <c r="I94" s="44"/>
       <c r="J94" s="51"/>
@@ -39263,13 +39269,13 @@
       </c>
       <c r="C95" s="44"/>
       <c r="D95" s="44">
-        <v>3.4049999999999998</v>
+        <v>3.3045</v>
       </c>
       <c r="E95" s="44">
-        <v>3.105</v>
+        <v>2.6695000000000002</v>
       </c>
       <c r="F95" s="44">
-        <v>1.0049999999999999</v>
+        <v>0.23449999999999999</v>
       </c>
       <c r="G95" s="44"/>
       <c r="H95" s="44"/>
@@ -39313,7 +39319,9 @@
       <c r="F97" s="44">
         <v>1.86</v>
       </c>
-      <c r="G97" s="44"/>
+      <c r="G97" s="44">
+        <v>15.251125</v>
+      </c>
       <c r="H97" s="44"/>
       <c r="I97" s="44"/>
       <c r="J97" s="51"/>
@@ -39347,16 +39355,16 @@
       </c>
       <c r="C99" s="44"/>
       <c r="D99" s="44">
-        <v>0.66500000000000004</v>
+        <v>0.66922999999999999</v>
       </c>
       <c r="E99" s="44">
-        <v>0.66949999999999998</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="F99" s="44">
-        <v>0.66949999999999998</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="G99" s="44">
-        <v>0.66949999999999998</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="H99" s="44"/>
       <c r="I99" s="44"/>
@@ -39373,16 +39381,16 @@
       </c>
       <c r="C100" s="44"/>
       <c r="D100" s="44">
-        <v>1.9370000000000001</v>
+        <v>1.9580500000000001</v>
       </c>
       <c r="E100" s="44">
-        <v>7.9045759999999996</v>
+        <v>12.095198</v>
       </c>
       <c r="F100" s="44">
-        <v>33.876519000000002</v>
+        <v>47.305767000000003</v>
       </c>
       <c r="G100" s="44">
-        <v>56.930736000000003</v>
+        <v>84.990144000000001</v>
       </c>
       <c r="H100" s="44"/>
       <c r="I100" s="44"/>
@@ -39399,16 +39407,16 @@
       </c>
       <c r="C101" s="44"/>
       <c r="D101" s="44">
-        <v>1.768</v>
+        <v>1.78064</v>
       </c>
       <c r="E101" s="44">
-        <v>17.569557</v>
+        <v>9.5041530000000005</v>
       </c>
       <c r="F101" s="44">
-        <v>34.940035000000002</v>
+        <v>30.965987999999999</v>
       </c>
       <c r="G101" s="44">
-        <v>46.356721999999998</v>
+        <v>51.072966999999998</v>
       </c>
       <c r="H101" s="44"/>
       <c r="I101" s="44"/>
@@ -39425,15 +39433,17 @@
       </c>
       <c r="C102" s="44"/>
       <c r="D102" s="44">
-        <v>1.234</v>
+        <v>1.167592</v>
       </c>
       <c r="E102" s="44">
-        <v>1.6339999999999999</v>
+        <v>10.202121</v>
       </c>
       <c r="F102" s="44">
-        <v>1.3985000000000001</v>
-      </c>
-      <c r="G102" s="44"/>
+        <v>10.057760999999999</v>
+      </c>
+      <c r="G102" s="44">
+        <v>33.780811999999997</v>
+      </c>
       <c r="H102" s="44"/>
       <c r="I102" s="44"/>
       <c r="J102" s="51"/>
@@ -39450,8 +39460,12 @@
       <c r="C103" s="44"/>
       <c r="D103" s="44"/>
       <c r="E103" s="44"/>
-      <c r="F103" s="44"/>
-      <c r="G103" s="44"/>
+      <c r="F103" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="G103" s="44">
+        <v>0.8</v>
+      </c>
       <c r="H103" s="44"/>
       <c r="I103" s="44"/>
       <c r="J103" s="51"/>
@@ -39503,16 +39517,16 @@
       </c>
       <c r="C106" s="44"/>
       <c r="D106" s="44">
-        <v>2.9</v>
+        <v>2.8208000000000002</v>
       </c>
       <c r="E106" s="44">
-        <v>4.5078800000000001</v>
+        <v>2.5568</v>
       </c>
       <c r="F106" s="44">
-        <v>4.5478610000000002</v>
+        <v>5.6</v>
       </c>
       <c r="G106" s="44">
-        <v>6.5169779999999999</v>
+        <v>5.6</v>
       </c>
       <c r="H106" s="44"/>
       <c r="I106" s="44"/>
@@ -39533,19 +39547,19 @@
       </c>
       <c r="D107" s="150">
         <f t="shared" si="12"/>
-        <v>53.149000000000001</v>
+        <v>49.780111999999995</v>
       </c>
       <c r="E107" s="150">
         <f t="shared" si="12"/>
-        <v>72.380677999999989</v>
+        <v>61.690406000000003</v>
       </c>
       <c r="F107" s="150">
         <f t="shared" si="12"/>
-        <v>127.33097999999998</v>
+        <v>107.03598199999999</v>
       </c>
       <c r="G107" s="150">
         <f t="shared" si="12"/>
-        <v>178.51986899999997</v>
+        <v>204.43488400000001</v>
       </c>
       <c r="H107" s="150">
         <f t="shared" si="12"/>
@@ -39583,9 +39597,7 @@
         <v>1327</v>
       </c>
       <c r="C109" s="44"/>
-      <c r="D109" s="44">
-        <v>2.1440000000000001</v>
-      </c>
+      <c r="D109" s="44"/>
       <c r="E109" s="44"/>
       <c r="F109" s="44"/>
       <c r="G109" s="44"/>
@@ -39622,15 +39634,9 @@
       </c>
       <c r="C111" s="44"/>
       <c r="D111" s="44"/>
-      <c r="E111" s="44">
-        <v>3.6431239999999998</v>
-      </c>
-      <c r="F111" s="44">
-        <v>3.2508010000000001</v>
-      </c>
-      <c r="G111" s="44">
-        <v>5.0797990000000004</v>
-      </c>
+      <c r="E111" s="44"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="44"/>
       <c r="H111" s="44"/>
       <c r="I111" s="44"/>
       <c r="J111" s="51"/>
@@ -39754,12 +39760,8 @@
       </c>
       <c r="C118" s="44"/>
       <c r="D118" s="44"/>
-      <c r="E118" s="44">
-        <v>3.7150430000000001</v>
-      </c>
-      <c r="F118" s="44">
-        <v>4.169359</v>
-      </c>
+      <c r="E118" s="44"/>
+      <c r="F118" s="44"/>
       <c r="G118" s="44"/>
       <c r="H118" s="44"/>
       <c r="I118" s="44"/>
@@ -39793,18 +39795,10 @@
         <v>1327</v>
       </c>
       <c r="C120" s="44"/>
-      <c r="D120" s="44">
-        <v>0.35</v>
-      </c>
-      <c r="E120" s="44">
-        <v>5</v>
-      </c>
-      <c r="F120" s="44">
-        <v>1.2716289999999999</v>
-      </c>
-      <c r="G120" s="44">
-        <v>1.5393730000000001</v>
-      </c>
+      <c r="D120" s="44"/>
+      <c r="E120" s="44"/>
+      <c r="F120" s="44"/>
+      <c r="G120" s="44"/>
       <c r="H120" s="44"/>
       <c r="I120" s="44"/>
       <c r="J120" s="51"/>
@@ -39875,12 +39869,8 @@
       <c r="C124" s="44"/>
       <c r="D124" s="44"/>
       <c r="E124" s="44"/>
-      <c r="F124" s="44">
-        <v>0.40296500000000002</v>
-      </c>
-      <c r="G124" s="44">
-        <v>0.216171</v>
-      </c>
+      <c r="F124" s="44"/>
+      <c r="G124" s="44"/>
       <c r="H124" s="44"/>
       <c r="I124" s="44"/>
       <c r="J124" s="51"/>
@@ -39900,19 +39890,19 @@
       </c>
       <c r="D125" s="150">
         <f t="shared" si="13"/>
-        <v>2.4940000000000002</v>
+        <v>0</v>
       </c>
       <c r="E125" s="150">
         <f t="shared" si="13"/>
-        <v>12.358167</v>
+        <v>0</v>
       </c>
       <c r="F125" s="150">
         <f t="shared" si="13"/>
-        <v>9.094754</v>
+        <v>0</v>
       </c>
       <c r="G125" s="150">
         <f t="shared" si="13"/>
-        <v>6.8353430000000008</v>
+        <v>0</v>
       </c>
       <c r="H125" s="150">
         <f t="shared" si="13"/>
@@ -40312,16 +40302,16 @@
       </c>
       <c r="C146" s="44"/>
       <c r="D146" s="44">
-        <v>2.1348940000000001</v>
+        <v>2.0050569999999999</v>
       </c>
       <c r="E146" s="44">
-        <v>1.6749369999999999</v>
+        <v>1.3631709999999999</v>
       </c>
       <c r="F146" s="44">
-        <v>1.1410670000000001</v>
+        <v>0.17097399999999999</v>
       </c>
       <c r="G146" s="44">
-        <v>0.35058899999999998</v>
+        <v>3.408E-3</v>
       </c>
       <c r="H146" s="44"/>
       <c r="I146" s="44"/>
@@ -40338,16 +40328,16 @@
       </c>
       <c r="C147" s="44"/>
       <c r="D147" s="44">
-        <v>2.0825E-2</v>
+        <v>9.887E-3</v>
       </c>
       <c r="E147" s="44">
-        <v>4.5185999999999997E-2</v>
+        <v>1.0654E-2</v>
       </c>
       <c r="F147" s="44">
-        <v>0.217831</v>
+        <v>5.0029999999999998E-2</v>
       </c>
       <c r="G147" s="44">
-        <v>1.0668629999999999</v>
+        <v>9.2887999999999998E-2</v>
       </c>
       <c r="H147" s="44"/>
       <c r="I147" s="44"/>
@@ -40382,16 +40372,16 @@
       </c>
       <c r="C149" s="44"/>
       <c r="D149" s="44">
-        <v>2.1132999999999999E-2</v>
+        <v>1.9498999999999999E-2</v>
       </c>
       <c r="E149" s="44">
-        <v>1.8741000000000001E-2</v>
+        <v>1.3676000000000001E-2</v>
       </c>
       <c r="F149" s="44">
-        <v>1.3738E-2</v>
+        <v>2.5829999999999998E-3</v>
       </c>
       <c r="G149" s="44">
-        <v>2.127E-3</v>
+        <v>1.8E-5</v>
       </c>
       <c r="H149" s="44"/>
       <c r="I149" s="44"/>
@@ -40434,7 +40424,9 @@
       <c r="F151" s="44">
         <v>0.15495700000000001</v>
       </c>
-      <c r="G151" s="44"/>
+      <c r="G151" s="44">
+        <v>1.1747570000000001</v>
+      </c>
       <c r="H151" s="44"/>
       <c r="I151" s="44"/>
       <c r="J151" s="51"/>
@@ -40451,8 +40443,12 @@
       <c r="C152" s="44"/>
       <c r="D152" s="44"/>
       <c r="E152" s="44"/>
-      <c r="F152" s="44"/>
-      <c r="G152" s="44"/>
+      <c r="F152" s="44">
+        <v>4.2230999999999998E-2</v>
+      </c>
+      <c r="G152" s="44">
+        <v>4.7654000000000002E-2</v>
+      </c>
       <c r="H152" s="44"/>
       <c r="I152" s="44"/>
       <c r="J152" s="51"/>
@@ -40526,19 +40522,19 @@
       </c>
       <c r="D156" s="150">
         <f t="shared" si="15"/>
-        <v>2.3311119999999996</v>
+        <v>2.1887029999999998</v>
       </c>
       <c r="E156" s="150">
         <f t="shared" si="15"/>
-        <v>1.8938209999999998</v>
+        <v>1.5424579999999999</v>
       </c>
       <c r="F156" s="150">
         <f t="shared" si="15"/>
-        <v>1.527593</v>
+        <v>0.42077500000000001</v>
       </c>
       <c r="G156" s="150">
         <f t="shared" si="15"/>
-        <v>1.4195789999999999</v>
+        <v>1.3187250000000001</v>
       </c>
       <c r="H156" s="150">
         <f t="shared" si="15"/>
@@ -40561,16 +40557,16 @@
       </c>
       <c r="C157" s="44"/>
       <c r="D157" s="44">
-        <v>113.176</v>
+        <v>0.10635500000000001</v>
       </c>
       <c r="E157" s="44">
-        <v>90.694999999999993</v>
+        <v>7.4650999999999995E-2</v>
       </c>
       <c r="F157" s="44">
-        <v>61.657999999999987</v>
+        <v>9.5490000000000002E-3</v>
       </c>
       <c r="G157" s="44">
-        <v>18.882999999999999</v>
+        <v>1.83E-4</v>
       </c>
       <c r="H157" s="44"/>
       <c r="I157" s="44"/>
@@ -40721,6 +40717,68 @@
       <c r="J165" s="51"/>
       <c r="K165" s="51"/>
       <c r="L165" s="51"/>
+    </row>
+    <row r="174" spans="1:12">
+      <c r="G174">
+        <v>3.5178579999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="4:7">
+      <c r="G177">
+        <v>5.6482570000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="4:7">
+      <c r="E179">
+        <v>6.6699999999999997E-3</v>
+      </c>
+      <c r="F179">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="G179">
+        <v>9.0000000000000006E-5</v>
+      </c>
+    </row>
+    <row r="180" spans="4:7">
+      <c r="E180">
+        <v>2.0752820000000001</v>
+      </c>
+      <c r="F180">
+        <v>5.3827480000000003</v>
+      </c>
+      <c r="G180">
+        <v>6.2242129999999998</v>
+      </c>
+    </row>
+    <row r="181" spans="4:7">
+      <c r="E181">
+        <v>1.169791</v>
+      </c>
+      <c r="F181">
+        <v>3.272618</v>
+      </c>
+      <c r="G181">
+        <v>2.4883280000000001</v>
+      </c>
+    </row>
+    <row r="182" spans="4:7">
+      <c r="D182">
+        <v>0.35</v>
+      </c>
+      <c r="E182">
+        <v>9.1943999999999998E-2</v>
+      </c>
+      <c r="G182">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="4:7">
+      <c r="F186">
+        <v>0.79109099999999999</v>
+      </c>
+      <c r="G186">
+        <v>2.64E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PWR sector final corrections done + added NCAP adjustor
</commit_message>
<xml_diff>
--- a/input/WB1.xlsx
+++ b/input/WB1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DDPTemplateAutomationV2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE98A4C-A824-41F2-87D1-8A8D7D64E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28403224-79B5-4CCC-8B04-AFE7603CFDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="888" firstSheet="12" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4474,10 +4474,10 @@
     <t>New installed capacities for the period (X-10; X)</t>
   </si>
   <si>
+    <t>Manual input</t>
+  </si>
+  <si>
     <t>Removed capacities for the period (X-10; X)</t>
-  </si>
-  <si>
-    <t>ignore</t>
   </si>
   <si>
     <t>Primary energies</t>
@@ -6027,7 +6027,7 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -6415,6 +6415,7 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="2" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -8331,23 +8332,23 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:17" ht="268.5" customHeight="1">
-      <c r="A4" s="226" t="s">
+      <c r="A4" s="227" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="227"/>
-      <c r="C4" s="227"/>
-      <c r="D4" s="227"/>
-      <c r="E4" s="227"/>
-      <c r="F4" s="227"/>
-      <c r="G4" s="227"/>
-      <c r="H4" s="227"/>
-      <c r="I4" s="227"/>
-      <c r="J4" s="227"/>
-      <c r="K4" s="227"/>
-      <c r="L4" s="227"/>
-      <c r="M4" s="227"/>
-      <c r="N4" s="227"/>
-      <c r="O4" s="228"/>
+      <c r="B4" s="228"/>
+      <c r="C4" s="228"/>
+      <c r="D4" s="228"/>
+      <c r="E4" s="228"/>
+      <c r="F4" s="228"/>
+      <c r="G4" s="228"/>
+      <c r="H4" s="228"/>
+      <c r="I4" s="228"/>
+      <c r="J4" s="228"/>
+      <c r="K4" s="228"/>
+      <c r="L4" s="228"/>
+      <c r="M4" s="228"/>
+      <c r="N4" s="228"/>
+      <c r="O4" s="229"/>
       <c r="Q4" s="177"/>
     </row>
     <row r="5" spans="1:17">
@@ -8368,23 +8369,23 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:17" ht="289.5" customHeight="1">
-      <c r="A6" s="226" t="s">
+      <c r="A6" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="227"/>
-      <c r="C6" s="227"/>
-      <c r="D6" s="227"/>
-      <c r="E6" s="227"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="227"/>
-      <c r="H6" s="227"/>
-      <c r="I6" s="227"/>
-      <c r="J6" s="227"/>
-      <c r="K6" s="227"/>
-      <c r="L6" s="227"/>
-      <c r="M6" s="227"/>
-      <c r="N6" s="227"/>
-      <c r="O6" s="228"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="228"/>
+      <c r="I6" s="228"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="228"/>
+      <c r="L6" s="228"/>
+      <c r="M6" s="228"/>
+      <c r="N6" s="228"/>
+      <c r="O6" s="229"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="5"/>
@@ -8421,23 +8422,23 @@
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:17" ht="21" customHeight="1">
-      <c r="A9" s="229" t="s">
+      <c r="A9" s="230" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="230"/>
-      <c r="C9" s="230"/>
-      <c r="D9" s="230"/>
-      <c r="E9" s="230"/>
-      <c r="F9" s="230"/>
-      <c r="G9" s="230"/>
-      <c r="H9" s="230"/>
-      <c r="I9" s="230"/>
-      <c r="J9" s="230"/>
-      <c r="K9" s="230"/>
-      <c r="L9" s="230"/>
-      <c r="M9" s="230"/>
-      <c r="N9" s="230"/>
-      <c r="O9" s="231"/>
+      <c r="B9" s="231"/>
+      <c r="C9" s="231"/>
+      <c r="D9" s="231"/>
+      <c r="E9" s="231"/>
+      <c r="F9" s="231"/>
+      <c r="G9" s="231"/>
+      <c r="H9" s="231"/>
+      <c r="I9" s="231"/>
+      <c r="J9" s="231"/>
+      <c r="K9" s="231"/>
+      <c r="L9" s="231"/>
+      <c r="M9" s="231"/>
+      <c r="N9" s="231"/>
+      <c r="O9" s="232"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="148"/>
@@ -8807,23 +8808,23 @@
       <c r="O28" s="7"/>
     </row>
     <row r="29" spans="1:15" ht="54" customHeight="1">
-      <c r="A29" s="219" t="s">
+      <c r="A29" s="220" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="220"/>
-      <c r="C29" s="220"/>
-      <c r="D29" s="220"/>
-      <c r="E29" s="220"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
-      <c r="K29" s="220"/>
-      <c r="L29" s="220"/>
-      <c r="M29" s="220"/>
-      <c r="N29" s="220"/>
-      <c r="O29" s="221"/>
+      <c r="B29" s="221"/>
+      <c r="C29" s="221"/>
+      <c r="D29" s="221"/>
+      <c r="E29" s="221"/>
+      <c r="F29" s="221"/>
+      <c r="G29" s="221"/>
+      <c r="H29" s="221"/>
+      <c r="I29" s="221"/>
+      <c r="J29" s="221"/>
+      <c r="K29" s="221"/>
+      <c r="L29" s="221"/>
+      <c r="M29" s="221"/>
+      <c r="N29" s="221"/>
+      <c r="O29" s="222"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="9"/>
@@ -8881,23 +8882,23 @@
       <c r="O32" s="7"/>
     </row>
     <row r="33" spans="1:15" ht="60" customHeight="1">
-      <c r="A33" s="219" t="s">
+      <c r="A33" s="220" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="220"/>
-      <c r="C33" s="220"/>
-      <c r="D33" s="220"/>
-      <c r="E33" s="220"/>
-      <c r="F33" s="220"/>
-      <c r="G33" s="220"/>
-      <c r="H33" s="220"/>
-      <c r="I33" s="220"/>
-      <c r="J33" s="220"/>
-      <c r="K33" s="220"/>
-      <c r="L33" s="220"/>
-      <c r="M33" s="220"/>
-      <c r="N33" s="220"/>
-      <c r="O33" s="221"/>
+      <c r="B33" s="221"/>
+      <c r="C33" s="221"/>
+      <c r="D33" s="221"/>
+      <c r="E33" s="221"/>
+      <c r="F33" s="221"/>
+      <c r="G33" s="221"/>
+      <c r="H33" s="221"/>
+      <c r="I33" s="221"/>
+      <c r="J33" s="221"/>
+      <c r="K33" s="221"/>
+      <c r="L33" s="221"/>
+      <c r="M33" s="221"/>
+      <c r="N33" s="221"/>
+      <c r="O33" s="222"/>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="145"/>
@@ -8950,7 +8951,7 @@
       </c>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="222" t="s">
+      <c r="A39" s="223" t="s">
         <v>29</v>
       </c>
       <c r="B39" s="173" t="s">
@@ -8961,7 +8962,7 @@
       </c>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="223"/>
+      <c r="A40" s="224"/>
       <c r="B40" s="173" t="s">
         <v>31</v>
       </c>
@@ -8970,7 +8971,7 @@
       </c>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="224"/>
+      <c r="A41" s="225"/>
       <c r="B41" s="173" t="s">
         <v>32</v>
       </c>
@@ -8979,7 +8980,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A42" s="225" t="s">
+      <c r="A42" s="226" t="s">
         <v>34</v>
       </c>
       <c r="B42" s="174" t="s">
@@ -8990,7 +8991,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A43" s="223"/>
+      <c r="A43" s="224"/>
       <c r="B43" s="174" t="s">
         <v>37</v>
       </c>
@@ -8999,7 +9000,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A44" s="223"/>
+      <c r="A44" s="224"/>
       <c r="B44" s="174" t="s">
         <v>39</v>
       </c>
@@ -9008,7 +9009,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A45" s="223"/>
+      <c r="A45" s="224"/>
       <c r="B45" s="174" t="s">
         <v>41</v>
       </c>
@@ -9017,7 +9018,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A46" s="223"/>
+      <c r="A46" s="224"/>
       <c r="B46" s="174" t="s">
         <v>43</v>
       </c>
@@ -9026,7 +9027,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A47" s="223"/>
+      <c r="A47" s="224"/>
       <c r="B47" s="174" t="s">
         <v>45</v>
       </c>
@@ -9035,7 +9036,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A48" s="223"/>
+      <c r="A48" s="224"/>
       <c r="B48" s="174" t="s">
         <v>47</v>
       </c>
@@ -9044,7 +9045,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A49" s="223"/>
+      <c r="A49" s="224"/>
       <c r="B49" s="174" t="s">
         <v>49</v>
       </c>
@@ -9053,7 +9054,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A50" s="223"/>
+      <c r="A50" s="224"/>
       <c r="B50" s="174" t="s">
         <v>50</v>
       </c>
@@ -9062,7 +9063,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A51" s="224"/>
+      <c r="A51" s="225"/>
       <c r="B51" s="174" t="s">
         <v>52</v>
       </c>
@@ -13296,10 +13297,10 @@
       <c r="I207" s="97"/>
     </row>
     <row r="208" spans="1:12">
-      <c r="A208" s="236" t="s">
+      <c r="A208" s="237" t="s">
         <v>623</v>
       </c>
-      <c r="B208" s="228"/>
+      <c r="B208" s="229"/>
       <c r="C208" s="103"/>
       <c r="D208" s="103"/>
       <c r="E208" s="103"/>
@@ -13309,10 +13310,10 @@
       <c r="I208" s="103"/>
     </row>
     <row r="209" spans="1:10">
-      <c r="A209" s="232" t="s">
+      <c r="A209" s="233" t="s">
         <v>822</v>
       </c>
-      <c r="B209" s="228"/>
+      <c r="B209" s="229"/>
       <c r="C209" s="103"/>
       <c r="D209" s="103"/>
       <c r="E209" s="103"/>
@@ -13322,10 +13323,10 @@
       <c r="I209" s="103"/>
     </row>
     <row r="210" spans="1:10">
-      <c r="A210" s="232" t="s">
+      <c r="A210" s="233" t="s">
         <v>823</v>
       </c>
-      <c r="B210" s="228"/>
+      <c r="B210" s="229"/>
       <c r="C210" s="103"/>
       <c r="D210" s="103"/>
       <c r="E210" s="103"/>
@@ -13335,10 +13336,10 @@
       <c r="I210" s="103"/>
     </row>
     <row r="211" spans="1:10">
-      <c r="A211" s="232" t="s">
+      <c r="A211" s="233" t="s">
         <v>824</v>
       </c>
-      <c r="B211" s="228"/>
+      <c r="B211" s="229"/>
       <c r="C211" s="103"/>
       <c r="D211" s="103"/>
       <c r="E211" s="103"/>
@@ -13348,10 +13349,10 @@
       <c r="I211" s="103"/>
     </row>
     <row r="212" spans="1:10">
-      <c r="A212" s="232" t="s">
+      <c r="A212" s="233" t="s">
         <v>631</v>
       </c>
-      <c r="B212" s="228"/>
+      <c r="B212" s="229"/>
       <c r="C212" s="103"/>
       <c r="D212" s="103"/>
       <c r="E212" s="103"/>
@@ -13361,10 +13362,10 @@
       <c r="I212" s="103"/>
     </row>
     <row r="213" spans="1:10">
-      <c r="A213" s="232" t="s">
+      <c r="A213" s="233" t="s">
         <v>632</v>
       </c>
-      <c r="B213" s="228"/>
+      <c r="B213" s="229"/>
       <c r="C213" s="103"/>
       <c r="D213" s="103"/>
       <c r="E213" s="103"/>
@@ -13374,10 +13375,10 @@
       <c r="I213" s="103"/>
     </row>
     <row r="214" spans="1:10">
-      <c r="A214" s="232" t="s">
+      <c r="A214" s="233" t="s">
         <v>633</v>
       </c>
-      <c r="B214" s="228"/>
+      <c r="B214" s="229"/>
       <c r="C214" s="103"/>
       <c r="D214" s="103"/>
       <c r="E214" s="103"/>
@@ -13387,10 +13388,10 @@
       <c r="I214" s="103"/>
     </row>
     <row r="215" spans="1:10">
-      <c r="A215" s="232" t="s">
+      <c r="A215" s="233" t="s">
         <v>825</v>
       </c>
-      <c r="B215" s="228"/>
+      <c r="B215" s="229"/>
       <c r="C215" s="103"/>
       <c r="D215" s="103"/>
       <c r="E215" s="103"/>
@@ -13400,10 +13401,10 @@
       <c r="I215" s="103"/>
     </row>
     <row r="216" spans="1:10">
-      <c r="A216" s="232" t="s">
+      <c r="A216" s="233" t="s">
         <v>826</v>
       </c>
-      <c r="B216" s="228"/>
+      <c r="B216" s="229"/>
       <c r="C216" s="103"/>
       <c r="D216" s="103"/>
       <c r="E216" s="103"/>
@@ -13413,8 +13414,8 @@
       <c r="I216" s="103"/>
     </row>
     <row r="217" spans="1:10">
-      <c r="A217" s="232"/>
-      <c r="B217" s="228"/>
+      <c r="A217" s="233"/>
+      <c r="B217" s="229"/>
       <c r="C217" s="103"/>
       <c r="D217" s="103"/>
       <c r="E217" s="103"/>
@@ -13444,32 +13445,32 @@
       <c r="I219" s="97"/>
     </row>
     <row r="220" spans="1:10">
-      <c r="A220" s="235" t="s">
+      <c r="A220" s="236" t="s">
         <v>827</v>
       </c>
-      <c r="B220" s="220"/>
-      <c r="C220" s="220"/>
-      <c r="D220" s="220"/>
-      <c r="E220" s="220"/>
-      <c r="F220" s="220"/>
-      <c r="G220" s="220"/>
-      <c r="H220" s="220"/>
-      <c r="I220" s="220"/>
-      <c r="J220" s="220"/>
+      <c r="B220" s="221"/>
+      <c r="C220" s="221"/>
+      <c r="D220" s="221"/>
+      <c r="E220" s="221"/>
+      <c r="F220" s="221"/>
+      <c r="G220" s="221"/>
+      <c r="H220" s="221"/>
+      <c r="I220" s="221"/>
+      <c r="J220" s="221"/>
     </row>
     <row r="221" spans="1:10">
-      <c r="A221" s="234" t="s">
+      <c r="A221" s="235" t="s">
         <v>828</v>
       </c>
-      <c r="B221" s="220"/>
-      <c r="C221" s="220"/>
-      <c r="D221" s="220"/>
-      <c r="E221" s="220"/>
-      <c r="F221" s="220"/>
-      <c r="G221" s="220"/>
-      <c r="H221" s="220"/>
-      <c r="I221" s="220"/>
-      <c r="J221" s="220"/>
+      <c r="B221" s="221"/>
+      <c r="C221" s="221"/>
+      <c r="D221" s="221"/>
+      <c r="E221" s="221"/>
+      <c r="F221" s="221"/>
+      <c r="G221" s="221"/>
+      <c r="H221" s="221"/>
+      <c r="I221" s="221"/>
+      <c r="J221" s="221"/>
     </row>
     <row r="222" spans="1:10">
       <c r="A222" s="164"/>
@@ -13484,32 +13485,32 @@
       <c r="J222" s="104"/>
     </row>
     <row r="223" spans="1:10">
-      <c r="A223" s="235" t="s">
+      <c r="A223" s="236" t="s">
         <v>829</v>
       </c>
-      <c r="B223" s="220"/>
-      <c r="C223" s="220"/>
-      <c r="D223" s="220"/>
-      <c r="E223" s="220"/>
-      <c r="F223" s="220"/>
-      <c r="G223" s="220"/>
-      <c r="H223" s="220"/>
-      <c r="I223" s="220"/>
-      <c r="J223" s="220"/>
+      <c r="B223" s="221"/>
+      <c r="C223" s="221"/>
+      <c r="D223" s="221"/>
+      <c r="E223" s="221"/>
+      <c r="F223" s="221"/>
+      <c r="G223" s="221"/>
+      <c r="H223" s="221"/>
+      <c r="I223" s="221"/>
+      <c r="J223" s="221"/>
     </row>
     <row r="224" spans="1:10">
-      <c r="A224" s="234" t="s">
+      <c r="A224" s="235" t="s">
         <v>830</v>
       </c>
-      <c r="B224" s="220"/>
-      <c r="C224" s="220"/>
-      <c r="D224" s="220"/>
-      <c r="E224" s="220"/>
-      <c r="F224" s="220"/>
-      <c r="G224" s="220"/>
-      <c r="H224" s="220"/>
-      <c r="I224" s="220"/>
-      <c r="J224" s="220"/>
+      <c r="B224" s="221"/>
+      <c r="C224" s="221"/>
+      <c r="D224" s="221"/>
+      <c r="E224" s="221"/>
+      <c r="F224" s="221"/>
+      <c r="G224" s="221"/>
+      <c r="H224" s="221"/>
+      <c r="I224" s="221"/>
+      <c r="J224" s="221"/>
     </row>
     <row r="225" spans="1:10">
       <c r="A225" s="164"/>
@@ -13524,32 +13525,32 @@
       <c r="J225" s="104"/>
     </row>
     <row r="226" spans="1:10">
-      <c r="A226" s="235" t="s">
+      <c r="A226" s="236" t="s">
         <v>831</v>
       </c>
-      <c r="B226" s="220"/>
-      <c r="C226" s="220"/>
-      <c r="D226" s="220"/>
-      <c r="E226" s="220"/>
-      <c r="F226" s="220"/>
-      <c r="G226" s="220"/>
-      <c r="H226" s="220"/>
-      <c r="I226" s="220"/>
-      <c r="J226" s="220"/>
+      <c r="B226" s="221"/>
+      <c r="C226" s="221"/>
+      <c r="D226" s="221"/>
+      <c r="E226" s="221"/>
+      <c r="F226" s="221"/>
+      <c r="G226" s="221"/>
+      <c r="H226" s="221"/>
+      <c r="I226" s="221"/>
+      <c r="J226" s="221"/>
     </row>
     <row r="227" spans="1:10">
-      <c r="A227" s="234" t="s">
+      <c r="A227" s="235" t="s">
         <v>832</v>
       </c>
-      <c r="B227" s="220"/>
-      <c r="C227" s="220"/>
-      <c r="D227" s="220"/>
-      <c r="E227" s="220"/>
-      <c r="F227" s="220"/>
-      <c r="G227" s="220"/>
-      <c r="H227" s="220"/>
-      <c r="I227" s="220"/>
-      <c r="J227" s="220"/>
+      <c r="B227" s="221"/>
+      <c r="C227" s="221"/>
+      <c r="D227" s="221"/>
+      <c r="E227" s="221"/>
+      <c r="F227" s="221"/>
+      <c r="G227" s="221"/>
+      <c r="H227" s="221"/>
+      <c r="I227" s="221"/>
+      <c r="J227" s="221"/>
     </row>
     <row r="228" spans="1:10">
       <c r="B228" s="97"/>
@@ -13562,32 +13563,32 @@
       <c r="I228" s="97"/>
     </row>
     <row r="229" spans="1:10">
-      <c r="A229" s="235" t="s">
+      <c r="A229" s="236" t="s">
         <v>833</v>
       </c>
-      <c r="B229" s="220"/>
-      <c r="C229" s="220"/>
-      <c r="D229" s="220"/>
-      <c r="E229" s="220"/>
-      <c r="F229" s="220"/>
-      <c r="G229" s="220"/>
-      <c r="H229" s="220"/>
-      <c r="I229" s="220"/>
-      <c r="J229" s="220"/>
+      <c r="B229" s="221"/>
+      <c r="C229" s="221"/>
+      <c r="D229" s="221"/>
+      <c r="E229" s="221"/>
+      <c r="F229" s="221"/>
+      <c r="G229" s="221"/>
+      <c r="H229" s="221"/>
+      <c r="I229" s="221"/>
+      <c r="J229" s="221"/>
     </row>
     <row r="230" spans="1:10">
-      <c r="A230" s="234" t="s">
+      <c r="A230" s="235" t="s">
         <v>834</v>
       </c>
-      <c r="B230" s="220"/>
-      <c r="C230" s="220"/>
-      <c r="D230" s="220"/>
-      <c r="E230" s="220"/>
-      <c r="F230" s="220"/>
-      <c r="G230" s="220"/>
-      <c r="H230" s="220"/>
-      <c r="I230" s="220"/>
-      <c r="J230" s="220"/>
+      <c r="B230" s="221"/>
+      <c r="C230" s="221"/>
+      <c r="D230" s="221"/>
+      <c r="E230" s="221"/>
+      <c r="F230" s="221"/>
+      <c r="G230" s="221"/>
+      <c r="H230" s="221"/>
+      <c r="I230" s="221"/>
+      <c r="J230" s="221"/>
     </row>
     <row r="231" spans="1:10">
       <c r="B231" s="97"/>
@@ -13600,32 +13601,32 @@
       <c r="I231" s="97"/>
     </row>
     <row r="232" spans="1:10">
-      <c r="A232" s="235" t="s">
+      <c r="A232" s="236" t="s">
         <v>636</v>
       </c>
-      <c r="B232" s="220"/>
-      <c r="C232" s="220"/>
-      <c r="D232" s="220"/>
-      <c r="E232" s="220"/>
-      <c r="F232" s="220"/>
-      <c r="G232" s="220"/>
-      <c r="H232" s="220"/>
-      <c r="I232" s="220"/>
-      <c r="J232" s="220"/>
+      <c r="B232" s="221"/>
+      <c r="C232" s="221"/>
+      <c r="D232" s="221"/>
+      <c r="E232" s="221"/>
+      <c r="F232" s="221"/>
+      <c r="G232" s="221"/>
+      <c r="H232" s="221"/>
+      <c r="I232" s="221"/>
+      <c r="J232" s="221"/>
     </row>
     <row r="233" spans="1:10">
-      <c r="A233" s="234" t="s">
+      <c r="A233" s="235" t="s">
         <v>835</v>
       </c>
-      <c r="B233" s="220"/>
-      <c r="C233" s="220"/>
-      <c r="D233" s="220"/>
-      <c r="E233" s="220"/>
-      <c r="F233" s="220"/>
-      <c r="G233" s="220"/>
-      <c r="H233" s="220"/>
-      <c r="I233" s="220"/>
-      <c r="J233" s="220"/>
+      <c r="B233" s="221"/>
+      <c r="C233" s="221"/>
+      <c r="D233" s="221"/>
+      <c r="E233" s="221"/>
+      <c r="F233" s="221"/>
+      <c r="G233" s="221"/>
+      <c r="H233" s="221"/>
+      <c r="I233" s="221"/>
+      <c r="J233" s="221"/>
     </row>
     <row r="234" spans="1:10">
       <c r="B234" s="97"/>
@@ -14069,22 +14070,22 @@
       <c r="E3" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="64.5" customHeight="1">
-      <c r="A5" s="239" t="s">
+      <c r="A5" s="240" t="s">
         <v>857</v>
       </c>
-      <c r="B5" s="227"/>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="228"/>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="229"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A7" s="237" t="s">
+      <c r="A7" s="238" t="s">
         <v>858</v>
       </c>
-      <c r="B7" s="238"/>
-      <c r="C7" s="238"/>
-      <c r="D7" s="238"/>
-      <c r="E7" s="238"/>
+      <c r="B7" s="239"/>
+      <c r="C7" s="239"/>
+      <c r="D7" s="239"/>
+      <c r="E7" s="239"/>
     </row>
     <row r="8" spans="1:5" ht="47.25" customHeight="1">
       <c r="A8" s="47" t="s">
@@ -14165,13 +14166,13 @@
       <c r="D14" s="167"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="238" t="s">
         <v>871</v>
       </c>
-      <c r="B15" s="238"/>
-      <c r="C15" s="238"/>
-      <c r="D15" s="238"/>
-      <c r="E15" s="238"/>
+      <c r="B15" s="239"/>
+      <c r="C15" s="239"/>
+      <c r="D15" s="239"/>
+      <c r="E15" s="239"/>
     </row>
     <row r="16" spans="1:5" ht="47.25" customHeight="1">
       <c r="A16" s="47" t="s">
@@ -14253,13 +14254,13 @@
       <c r="D22" s="167"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A23" s="237" t="s">
+      <c r="A23" s="238" t="s">
         <v>879</v>
       </c>
-      <c r="B23" s="238"/>
-      <c r="C23" s="238"/>
-      <c r="D23" s="238"/>
-      <c r="E23" s="238"/>
+      <c r="B23" s="239"/>
+      <c r="C23" s="239"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="239"/>
     </row>
     <row r="24" spans="1:6" ht="47.25" customHeight="1">
       <c r="A24" s="47" t="s">
@@ -14340,13 +14341,13 @@
       <c r="D30" s="167"/>
     </row>
     <row r="31" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A31" s="237" t="s">
+      <c r="A31" s="238" t="s">
         <v>885</v>
       </c>
-      <c r="B31" s="238"/>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
+      <c r="B31" s="239"/>
+      <c r="C31" s="239"/>
+      <c r="D31" s="239"/>
+      <c r="E31" s="239"/>
     </row>
     <row r="32" spans="1:6" ht="47.25" customHeight="1">
       <c r="A32" s="47" t="s">
@@ -14427,13 +14428,13 @@
       <c r="D38" s="167"/>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A39" s="237" t="s">
+      <c r="A39" s="238" t="s">
         <v>888</v>
       </c>
-      <c r="B39" s="238"/>
-      <c r="C39" s="238"/>
-      <c r="D39" s="238"/>
-      <c r="E39" s="238"/>
+      <c r="B39" s="239"/>
+      <c r="C39" s="239"/>
+      <c r="D39" s="239"/>
+      <c r="E39" s="239"/>
     </row>
     <row r="40" spans="1:5" ht="47.25" customHeight="1">
       <c r="A40" s="47" t="s">
@@ -21732,13 +21733,13 @@
       <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" ht="64.5" customHeight="1">
-      <c r="A5" s="239" t="s">
+      <c r="A5" s="240" t="s">
         <v>973</v>
       </c>
-      <c r="B5" s="227"/>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="228"/>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="229"/>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="B6" s="46"/>
@@ -37093,8 +37094,8 @@
   </sheetPr>
   <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="D27:G35"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N123" sqref="N123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -37193,21 +37194,21 @@
         <f t="shared" ref="C6:I6" si="0">C57/C21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D6" s="172" t="e">
+      <c r="D6" s="172">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="172" t="e">
+        <v>19.99449584120562</v>
+      </c>
+      <c r="E6" s="172">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="172" t="e">
+        <v>17.934055723644359</v>
+      </c>
+      <c r="F6" s="172">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" s="172" t="e">
+        <v>15.981711088304921</v>
+      </c>
+      <c r="G6" s="172">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>22.773966397334327</v>
       </c>
       <c r="H6" s="172" t="e">
         <f t="shared" si="0"/>
@@ -37231,19 +37232,19 @@
       </c>
       <c r="D7" s="172">
         <f t="shared" si="1"/>
-        <v>926.47334960024193</v>
+        <v>932.05356602699953</v>
       </c>
       <c r="E7" s="172">
         <f t="shared" si="1"/>
-        <v>604.13474807231455</v>
+        <v>603.48576699154637</v>
       </c>
       <c r="F7" s="172">
         <f t="shared" si="1"/>
-        <v>60.208162885254403</v>
+        <v>68.858149960678659</v>
       </c>
       <c r="G7" s="172">
         <f t="shared" si="1"/>
-        <v>0.5744964592361026</v>
+        <v>9.5874550673107173</v>
       </c>
       <c r="H7" s="172" t="e">
         <f t="shared" si="1"/>
@@ -37267,19 +37268,19 @@
       </c>
       <c r="D8" s="172">
         <f t="shared" si="2"/>
-        <v>205.88177100000004</v>
+        <v>209.23142200000001</v>
       </c>
       <c r="E8" s="172">
         <f t="shared" si="2"/>
-        <v>219.21848300000002</v>
+        <v>220.11551600000001</v>
       </c>
       <c r="F8" s="172">
         <f t="shared" si="2"/>
-        <v>277.89987600000001</v>
+        <v>282.56280500000003</v>
       </c>
       <c r="G8" s="172">
         <f t="shared" si="2"/>
-        <v>573.32642299999998</v>
+        <v>577.87744099999998</v>
       </c>
       <c r="H8" s="172">
         <f t="shared" si="2"/>
@@ -37303,19 +37304,19 @@
       </c>
       <c r="D9" s="172">
         <f t="shared" si="3"/>
-        <v>190.74397399999998</v>
+        <v>195.014893</v>
       </c>
       <c r="E9" s="172">
         <f t="shared" si="3"/>
-        <v>132.43750299999999</v>
+        <v>132.836581</v>
       </c>
       <c r="F9" s="172">
         <f t="shared" si="3"/>
-        <v>16.731840999999999</v>
+        <v>19.456752000000002</v>
       </c>
       <c r="G9" s="172">
         <f t="shared" si="3"/>
-        <v>0.329374</v>
+        <v>5.5403739999999999</v>
       </c>
       <c r="H9" s="172">
         <f t="shared" si="3"/>
@@ -37387,7 +37388,7 @@
       </c>
       <c r="G11" s="172">
         <f t="shared" si="5"/>
-        <v>-2.2426750000000002</v>
+        <v>2.2426750000000002</v>
       </c>
       <c r="H11" s="172">
         <f t="shared" si="5"/>
@@ -37643,10 +37644,18 @@
         <v>294</v>
       </c>
       <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
+      <c r="D21" s="44">
+        <v>10.464451</v>
+      </c>
+      <c r="E21" s="44">
+        <v>12.273605</v>
+      </c>
+      <c r="F21" s="44">
+        <v>17.680385000000001</v>
+      </c>
+      <c r="G21" s="44">
+        <v>25.374475</v>
+      </c>
       <c r="H21" s="44"/>
       <c r="I21" s="44"/>
       <c r="J21" s="196" t="s">
@@ -37663,17 +37672,21 @@
         <v>1311</v>
       </c>
       <c r="C22" s="44"/>
-      <c r="D22" s="44">
-        <v>59.308689999999999</v>
-      </c>
-      <c r="E22" s="44">
-        <v>65.956090000000003</v>
-      </c>
-      <c r="F22" s="44">
-        <v>71.375305999999995</v>
-      </c>
-      <c r="G22" s="44">
-        <v>75.517909000000003</v>
+      <c r="D22" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!D8</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!E8</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!F8</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!G8</f>
+        <v>0</v>
       </c>
       <c r="H22" s="44"/>
       <c r="I22" s="44"/>
@@ -37691,10 +37704,22 @@
         <v>303</v>
       </c>
       <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
+      <c r="D23" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!D184</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!E184</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!F184</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!G184</f>
+        <v>0</v>
+      </c>
       <c r="H23" s="44"/>
       <c r="I23" s="44"/>
       <c r="J23" s="196" t="s">
@@ -37711,10 +37736,22 @@
         <v>280</v>
       </c>
       <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
+      <c r="D24" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!D33</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!E33</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!F33</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="219">
+        <f>'MACRO-DEMO_ECO (DB)'!G33</f>
+        <v>0</v>
+      </c>
       <c r="H24" s="44"/>
       <c r="I24" s="44"/>
       <c r="J24" s="196" t="s">
@@ -37885,7 +37922,7 @@
         <v>54.762407000000003</v>
       </c>
       <c r="G31" s="44">
-        <v>93.838811000000007</v>
+        <v>95.800467999999995</v>
       </c>
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
@@ -38026,7 +38063,7 @@
       </c>
       <c r="G36" s="150">
         <f t="shared" si="7"/>
-        <v>501.21011000000004</v>
+        <v>503.17176699999999</v>
       </c>
       <c r="H36" s="150">
         <f t="shared" si="7"/>
@@ -38115,7 +38152,7 @@
       </c>
       <c r="C41" s="44"/>
       <c r="D41" s="44">
-        <v>177.6053</v>
+        <v>180.56411499999999</v>
       </c>
       <c r="E41" s="44">
         <v>125.686538</v>
@@ -38159,15 +38196,17 @@
       </c>
       <c r="C43" s="44"/>
       <c r="D43" s="44">
-        <v>0.70290600000000003</v>
+        <v>1.093742</v>
       </c>
       <c r="E43" s="44">
-        <v>0.44257099999999999</v>
+        <v>1.339604</v>
       </c>
       <c r="F43" s="44">
-        <v>0.18223500000000001</v>
-      </c>
-      <c r="G43" s="44"/>
+        <v>4.8451639999999996</v>
+      </c>
+      <c r="G43" s="44">
+        <v>4.551018</v>
+      </c>
       <c r="H43" s="44"/>
       <c r="I43" s="44"/>
       <c r="J43" s="51"/>
@@ -38473,19 +38512,19 @@
       </c>
       <c r="D57" s="150">
         <f t="shared" si="8"/>
-        <v>205.88177100000004</v>
+        <v>209.23142200000001</v>
       </c>
       <c r="E57" s="150">
         <f t="shared" si="8"/>
-        <v>219.21848300000002</v>
+        <v>220.11551600000001</v>
       </c>
       <c r="F57" s="150">
         <f t="shared" si="8"/>
-        <v>277.89987600000001</v>
+        <v>282.56280500000003</v>
       </c>
       <c r="G57" s="150">
         <f t="shared" si="8"/>
-        <v>573.32642299999998</v>
+        <v>577.87744099999998</v>
       </c>
       <c r="H57" s="150">
         <f t="shared" si="8"/>
@@ -38558,7 +38597,7 @@
       </c>
       <c r="C61" s="44"/>
       <c r="D61" s="44">
-        <v>189.77618899999999</v>
+        <v>193.80791600000001</v>
       </c>
       <c r="E61" s="44">
         <v>131.78553199999999</v>
@@ -38602,15 +38641,17 @@
       </c>
       <c r="C63" s="44"/>
       <c r="D63" s="44">
-        <v>0.31546400000000002</v>
+        <v>0.55465600000000004</v>
       </c>
       <c r="E63" s="44">
-        <v>0.198626</v>
+        <v>0.59770400000000001</v>
       </c>
       <c r="F63" s="44">
-        <v>8.1786999999999999E-2</v>
-      </c>
-      <c r="G63" s="44"/>
+        <v>2.8066979999999999</v>
+      </c>
+      <c r="G63" s="44">
+        <v>2.6785019999999999</v>
+      </c>
       <c r="H63" s="44"/>
       <c r="I63" s="44"/>
       <c r="J63" s="51"/>
@@ -38628,7 +38669,9 @@
       <c r="D64" s="44"/>
       <c r="E64" s="44"/>
       <c r="F64" s="44"/>
-      <c r="G64" s="44"/>
+      <c r="G64" s="44">
+        <v>2.5324979999999999</v>
+      </c>
       <c r="H64" s="44"/>
       <c r="I64" s="44"/>
       <c r="J64" s="51"/>
@@ -38870,19 +38913,19 @@
       </c>
       <c r="D77" s="150">
         <f t="shared" si="9"/>
-        <v>190.74397399999998</v>
+        <v>195.014893</v>
       </c>
       <c r="E77" s="150">
         <f t="shared" si="9"/>
-        <v>132.43750299999999</v>
+        <v>132.836581</v>
       </c>
       <c r="F77" s="150">
         <f t="shared" si="9"/>
-        <v>16.731840999999999</v>
+        <v>19.456752000000002</v>
       </c>
       <c r="G77" s="150">
         <f t="shared" si="9"/>
-        <v>0.329374</v>
+        <v>5.5403739999999999</v>
       </c>
       <c r="H77" s="150">
         <f t="shared" si="9"/>
@@ -39054,31 +39097,31 @@
         <v>953</v>
       </c>
       <c r="C86" s="150">
-        <f t="shared" ref="C86:I86" si="10">SUM(C81:C85)</f>
+        <f>SUM(C81:C85)</f>
         <v>0</v>
       </c>
       <c r="D86" s="150">
-        <f t="shared" si="10"/>
+        <f>ABS(SUM(D81:D85))</f>
         <v>0</v>
       </c>
       <c r="E86" s="150">
-        <f t="shared" si="10"/>
+        <f>ABS(SUM(E81:E85))</f>
         <v>0</v>
       </c>
       <c r="F86" s="150">
-        <f t="shared" si="10"/>
+        <f>ABS(SUM(F81:F85))</f>
         <v>0</v>
       </c>
       <c r="G86" s="150">
-        <f t="shared" si="10"/>
-        <v>-2.2426750000000002</v>
+        <f>ABS(SUM(G81:G85))</f>
+        <v>2.2426750000000002</v>
       </c>
       <c r="H86" s="150">
-        <f t="shared" si="10"/>
+        <f>SUM(H81:H85)</f>
         <v>0</v>
       </c>
       <c r="I86" s="150">
-        <f t="shared" si="10"/>
+        <f>SUM(I81:I85)</f>
         <v>0</v>
       </c>
       <c r="J86" s="51"/>
@@ -39109,31 +39152,31 @@
         <v>955</v>
       </c>
       <c r="C88" s="150">
-        <f t="shared" ref="C88:I88" si="11">C77+C79-C86</f>
+        <f t="shared" ref="C88:I88" si="10">C77+C79-C86</f>
         <v>0</v>
       </c>
       <c r="D88" s="150">
-        <f t="shared" si="11"/>
-        <v>191.54926899999998</v>
+        <f t="shared" si="10"/>
+        <v>195.820188</v>
       </c>
       <c r="E88" s="150">
-        <f t="shared" si="11"/>
-        <v>132.98531199999999</v>
+        <f t="shared" si="10"/>
+        <v>133.38439</v>
       </c>
       <c r="F88" s="150">
-        <f t="shared" si="11"/>
-        <v>16.803414</v>
+        <f t="shared" si="10"/>
+        <v>19.528325000000002</v>
       </c>
       <c r="G88" s="150">
-        <f t="shared" si="11"/>
-        <v>2.5784750000000001</v>
+        <f t="shared" si="10"/>
+        <v>3.304125</v>
       </c>
       <c r="H88" s="150">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I88" s="150">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J88" s="51"/>
@@ -39181,7 +39224,7 @@
       </c>
       <c r="C91" s="44"/>
       <c r="D91" s="44">
-        <v>36.064500000000002</v>
+        <v>36.526038</v>
       </c>
       <c r="E91" s="44">
         <v>22.030166999999999</v>
@@ -39225,15 +39268,17 @@
       </c>
       <c r="C93" s="44"/>
       <c r="D93" s="44">
-        <v>0.15479999999999999</v>
+        <v>0.37890000000000001</v>
       </c>
       <c r="E93" s="44">
-        <v>9.7466999999999998E-2</v>
+        <v>1.2875479999999999</v>
       </c>
       <c r="F93" s="44">
-        <v>4.0133000000000002E-2</v>
-      </c>
-      <c r="G93" s="44"/>
+        <v>9.2111680000000007</v>
+      </c>
+      <c r="G93" s="44">
+        <v>9.1129350000000002</v>
+      </c>
       <c r="H93" s="44"/>
       <c r="I93" s="44"/>
       <c r="J93" s="51"/>
@@ -39520,13 +39565,13 @@
         <v>2.8208000000000002</v>
       </c>
       <c r="E106" s="44">
-        <v>2.5568</v>
+        <v>3.631265</v>
       </c>
       <c r="F106" s="44">
-        <v>5.6</v>
+        <v>13.665908</v>
       </c>
       <c r="G106" s="44">
-        <v>5.6</v>
+        <v>32.475971999999999</v>
       </c>
       <c r="H106" s="44"/>
       <c r="I106" s="44"/>
@@ -39542,31 +39587,31 @@
         <v>1327</v>
       </c>
       <c r="C107" s="150">
-        <f t="shared" ref="C107:I107" si="12">SUM(C91:C106)</f>
+        <f t="shared" ref="C107:I107" si="11">SUM(C91:C106)</f>
         <v>0</v>
       </c>
       <c r="D107" s="150">
-        <f t="shared" si="12"/>
-        <v>49.780111999999995</v>
+        <f t="shared" si="11"/>
+        <v>50.465749999999993</v>
       </c>
       <c r="E107" s="150">
-        <f t="shared" si="12"/>
-        <v>61.690406000000003</v>
+        <f t="shared" si="11"/>
+        <v>63.954951999999999</v>
       </c>
       <c r="F107" s="150">
-        <f t="shared" si="12"/>
-        <v>107.03598199999999</v>
+        <f t="shared" si="11"/>
+        <v>124.272925</v>
       </c>
       <c r="G107" s="150">
-        <f t="shared" si="12"/>
-        <v>204.43488400000001</v>
+        <f t="shared" si="11"/>
+        <v>240.42379099999999</v>
       </c>
       <c r="H107" s="150">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I107" s="150">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J107" s="51"/>
@@ -39605,7 +39650,9 @@
       <c r="I109" s="44"/>
       <c r="J109" s="51"/>
       <c r="K109" s="51"/>
-      <c r="L109" s="51"/>
+      <c r="L109" s="206" t="s">
+        <v>1361</v>
+      </c>
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="22" t="s">
@@ -39634,9 +39681,15 @@
       </c>
       <c r="C111" s="44"/>
       <c r="D111" s="44"/>
-      <c r="E111" s="44"/>
-      <c r="F111" s="44"/>
-      <c r="G111" s="44"/>
+      <c r="E111" s="44">
+        <v>1.05</v>
+      </c>
+      <c r="F111" s="44">
+        <v>8.06</v>
+      </c>
+      <c r="G111" s="44">
+        <v>0</v>
+      </c>
       <c r="H111" s="44"/>
       <c r="I111" s="44"/>
       <c r="J111" s="51"/>
@@ -39652,9 +39705,15 @@
       </c>
       <c r="C112" s="44"/>
       <c r="D112" s="44"/>
-      <c r="E112" s="44"/>
-      <c r="F112" s="44"/>
-      <c r="G112" s="44"/>
+      <c r="E112" s="44">
+        <v>0</v>
+      </c>
+      <c r="F112" s="44">
+        <v>0</v>
+      </c>
+      <c r="G112" s="44">
+        <v>11.59</v>
+      </c>
       <c r="H112" s="44"/>
       <c r="I112" s="44"/>
       <c r="J112" s="51"/>
@@ -39706,9 +39765,15 @@
       </c>
       <c r="C115" s="44"/>
       <c r="D115" s="44"/>
-      <c r="E115" s="44"/>
-      <c r="F115" s="44"/>
-      <c r="G115" s="44"/>
+      <c r="E115" s="44">
+        <v>0</v>
+      </c>
+      <c r="F115" s="44">
+        <v>0</v>
+      </c>
+      <c r="G115" s="44">
+        <v>15.25</v>
+      </c>
       <c r="H115" s="44"/>
       <c r="I115" s="44"/>
       <c r="J115" s="51"/>
@@ -39742,9 +39807,15 @@
       </c>
       <c r="C117" s="44"/>
       <c r="D117" s="44"/>
-      <c r="E117" s="44"/>
-      <c r="F117" s="44"/>
-      <c r="G117" s="44"/>
+      <c r="E117" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="F117" s="44">
+        <v>0</v>
+      </c>
+      <c r="G117" s="44">
+        <v>0</v>
+      </c>
       <c r="H117" s="44"/>
       <c r="I117" s="44"/>
       <c r="J117" s="51"/>
@@ -39760,9 +39831,15 @@
       </c>
       <c r="C118" s="44"/>
       <c r="D118" s="44"/>
-      <c r="E118" s="44"/>
-      <c r="F118" s="44"/>
-      <c r="G118" s="44"/>
+      <c r="E118" s="44">
+        <v>10.92</v>
+      </c>
+      <c r="F118" s="44">
+        <v>36.380000000000003</v>
+      </c>
+      <c r="G118" s="44">
+        <v>48.61</v>
+      </c>
       <c r="H118" s="44"/>
       <c r="I118" s="44"/>
       <c r="J118" s="51"/>
@@ -39778,9 +39855,15 @@
       </c>
       <c r="C119" s="44"/>
       <c r="D119" s="44"/>
-      <c r="E119" s="44"/>
-      <c r="F119" s="44"/>
-      <c r="G119" s="44"/>
+      <c r="E119" s="44">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="F119" s="44">
+        <v>22.12</v>
+      </c>
+      <c r="G119" s="44">
+        <v>24.25</v>
+      </c>
       <c r="H119" s="44"/>
       <c r="I119" s="44"/>
       <c r="J119" s="51"/>
@@ -39796,9 +39879,15 @@
       </c>
       <c r="C120" s="44"/>
       <c r="D120" s="44"/>
-      <c r="E120" s="44"/>
-      <c r="F120" s="44"/>
-      <c r="G120" s="44"/>
+      <c r="E120" s="44">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="F120" s="44">
+        <v>0</v>
+      </c>
+      <c r="G120" s="44">
+        <v>33.119999999999997</v>
+      </c>
       <c r="H120" s="44"/>
       <c r="I120" s="44"/>
       <c r="J120" s="51"/>
@@ -39814,9 +39903,15 @@
       </c>
       <c r="C121" s="44"/>
       <c r="D121" s="44"/>
-      <c r="E121" s="44"/>
-      <c r="F121" s="44"/>
-      <c r="G121" s="44"/>
+      <c r="E121" s="44">
+        <v>0</v>
+      </c>
+      <c r="F121" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="G121" s="44">
+        <v>0</v>
+      </c>
       <c r="H121" s="44"/>
       <c r="I121" s="44"/>
       <c r="J121" s="51"/>
@@ -39868,9 +39963,15 @@
       </c>
       <c r="C124" s="44"/>
       <c r="D124" s="44"/>
-      <c r="E124" s="44"/>
-      <c r="F124" s="44"/>
-      <c r="G124" s="44"/>
+      <c r="E124" s="44">
+        <v>1.07</v>
+      </c>
+      <c r="F124" s="44">
+        <v>11.23</v>
+      </c>
+      <c r="G124" s="44">
+        <v>20.260000000000002</v>
+      </c>
       <c r="H124" s="44"/>
       <c r="I124" s="44"/>
       <c r="J124" s="51"/>
@@ -39885,31 +39986,31 @@
         <v>1327</v>
       </c>
       <c r="C125" s="150">
-        <f t="shared" ref="C125:I125" si="13">SUM(C109:C124)</f>
+        <f t="shared" ref="C125:I125" si="12">SUM(C109:C124)</f>
         <v>0</v>
       </c>
       <c r="D125" s="150">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E125" s="150">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>30.96</v>
       </c>
       <c r="F125" s="150">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>78.59</v>
       </c>
       <c r="G125" s="150">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>153.07999999999998</v>
       </c>
       <c r="H125" s="150">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I125" s="150">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J125" s="51"/>
@@ -39918,7 +40019,7 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="21" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="21"/>
@@ -39941,16 +40042,20 @@
       </c>
       <c r="C127" s="44"/>
       <c r="D127" s="44"/>
-      <c r="E127" s="44"/>
-      <c r="F127" s="44"/>
-      <c r="G127" s="44"/>
+      <c r="E127" s="44">
+        <v>14.5</v>
+      </c>
+      <c r="F127" s="44">
+        <v>12.53</v>
+      </c>
+      <c r="G127" s="44">
+        <v>8.83</v>
+      </c>
       <c r="H127" s="44"/>
       <c r="I127" s="44"/>
       <c r="J127" s="51"/>
       <c r="K127" s="51"/>
-      <c r="L127" s="206" t="s">
-        <v>1362</v>
-      </c>
+      <c r="L127" s="51"/>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="22" t="s">
@@ -39961,9 +40066,15 @@
       </c>
       <c r="C128" s="44"/>
       <c r="D128" s="44"/>
-      <c r="E128" s="44"/>
-      <c r="F128" s="44"/>
-      <c r="G128" s="44"/>
+      <c r="E128" s="44">
+        <v>0</v>
+      </c>
+      <c r="F128" s="44">
+        <v>0</v>
+      </c>
+      <c r="G128" s="44">
+        <v>0</v>
+      </c>
       <c r="H128" s="44"/>
       <c r="I128" s="44"/>
       <c r="J128" s="51"/>
@@ -39979,9 +40090,15 @@
       </c>
       <c r="C129" s="44"/>
       <c r="D129" s="44"/>
-      <c r="E129" s="44"/>
-      <c r="F129" s="44"/>
-      <c r="G129" s="44"/>
+      <c r="E129" s="44">
+        <v>0</v>
+      </c>
+      <c r="F129" s="44">
+        <v>0</v>
+      </c>
+      <c r="G129" s="44">
+        <v>0.1</v>
+      </c>
       <c r="H129" s="44"/>
       <c r="I129" s="44"/>
       <c r="J129" s="51"/>
@@ -39997,9 +40114,15 @@
       </c>
       <c r="C130" s="44"/>
       <c r="D130" s="44"/>
-      <c r="E130" s="44"/>
-      <c r="F130" s="44"/>
-      <c r="G130" s="44"/>
+      <c r="E130" s="44">
+        <v>0</v>
+      </c>
+      <c r="F130" s="44">
+        <v>0</v>
+      </c>
+      <c r="G130" s="44">
+        <v>0</v>
+      </c>
       <c r="H130" s="44"/>
       <c r="I130" s="44"/>
       <c r="J130" s="51"/>
@@ -40015,9 +40138,15 @@
       </c>
       <c r="C131" s="44"/>
       <c r="D131" s="44"/>
-      <c r="E131" s="44"/>
-      <c r="F131" s="44"/>
-      <c r="G131" s="44"/>
+      <c r="E131" s="44">
+        <v>0.64</v>
+      </c>
+      <c r="F131" s="44">
+        <v>2.44</v>
+      </c>
+      <c r="G131" s="44">
+        <v>0.23</v>
+      </c>
       <c r="H131" s="44"/>
       <c r="I131" s="44"/>
       <c r="J131" s="51"/>
@@ -40033,9 +40162,15 @@
       </c>
       <c r="C132" s="44"/>
       <c r="D132" s="44"/>
-      <c r="E132" s="44"/>
-      <c r="F132" s="44"/>
-      <c r="G132" s="44"/>
+      <c r="E132" s="44">
+        <v>0</v>
+      </c>
+      <c r="F132" s="44">
+        <v>0</v>
+      </c>
+      <c r="G132" s="44">
+        <v>0</v>
+      </c>
       <c r="H132" s="44"/>
       <c r="I132" s="44"/>
       <c r="J132" s="51"/>
@@ -40051,9 +40186,15 @@
       </c>
       <c r="C133" s="44"/>
       <c r="D133" s="44"/>
-      <c r="E133" s="44"/>
-      <c r="F133" s="44"/>
-      <c r="G133" s="44"/>
+      <c r="E133" s="44">
+        <v>0</v>
+      </c>
+      <c r="F133" s="44">
+        <v>0</v>
+      </c>
+      <c r="G133" s="44">
+        <v>0</v>
+      </c>
       <c r="H133" s="44"/>
       <c r="I133" s="44"/>
       <c r="J133" s="51"/>
@@ -40069,9 +40210,15 @@
       </c>
       <c r="C134" s="44"/>
       <c r="D134" s="44"/>
-      <c r="E134" s="44"/>
-      <c r="F134" s="44"/>
-      <c r="G134" s="44"/>
+      <c r="E134" s="44">
+        <v>0</v>
+      </c>
+      <c r="F134" s="44">
+        <v>0</v>
+      </c>
+      <c r="G134" s="44">
+        <v>0</v>
+      </c>
       <c r="H134" s="44"/>
       <c r="I134" s="44"/>
       <c r="J134" s="51"/>
@@ -40087,9 +40234,15 @@
       </c>
       <c r="C135" s="44"/>
       <c r="D135" s="44"/>
-      <c r="E135" s="44"/>
-      <c r="F135" s="44"/>
-      <c r="G135" s="44"/>
+      <c r="E135" s="44">
+        <v>0</v>
+      </c>
+      <c r="F135" s="44">
+        <v>0</v>
+      </c>
+      <c r="G135" s="44">
+        <v>0</v>
+      </c>
       <c r="H135" s="44"/>
       <c r="I135" s="44"/>
       <c r="J135" s="51"/>
@@ -40105,9 +40258,15 @@
       </c>
       <c r="C136" s="44"/>
       <c r="D136" s="44"/>
-      <c r="E136" s="44"/>
-      <c r="F136" s="44"/>
-      <c r="G136" s="44"/>
+      <c r="E136" s="44">
+        <v>0</v>
+      </c>
+      <c r="F136" s="44">
+        <v>0</v>
+      </c>
+      <c r="G136" s="44">
+        <v>0</v>
+      </c>
       <c r="H136" s="44"/>
       <c r="I136" s="44"/>
       <c r="J136" s="51"/>
@@ -40123,9 +40282,15 @@
       </c>
       <c r="C137" s="44"/>
       <c r="D137" s="44"/>
-      <c r="E137" s="44"/>
-      <c r="F137" s="44"/>
-      <c r="G137" s="44"/>
+      <c r="E137" s="44">
+        <v>0</v>
+      </c>
+      <c r="F137" s="44">
+        <v>0</v>
+      </c>
+      <c r="G137" s="44">
+        <v>0</v>
+      </c>
       <c r="H137" s="44"/>
       <c r="I137" s="44"/>
       <c r="J137" s="51"/>
@@ -40141,9 +40306,15 @@
       </c>
       <c r="C138" s="44"/>
       <c r="D138" s="44"/>
-      <c r="E138" s="44"/>
-      <c r="F138" s="44"/>
-      <c r="G138" s="44"/>
+      <c r="E138" s="44">
+        <v>0</v>
+      </c>
+      <c r="F138" s="44">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G138" s="44">
+        <v>0</v>
+      </c>
       <c r="H138" s="44"/>
       <c r="I138" s="44"/>
       <c r="J138" s="51"/>
@@ -40159,9 +40330,15 @@
       </c>
       <c r="C139" s="44"/>
       <c r="D139" s="44"/>
-      <c r="E139" s="44"/>
-      <c r="F139" s="44"/>
-      <c r="G139" s="44"/>
+      <c r="E139" s="44">
+        <v>0</v>
+      </c>
+      <c r="F139" s="44">
+        <v>0</v>
+      </c>
+      <c r="G139" s="44">
+        <v>0</v>
+      </c>
       <c r="H139" s="44"/>
       <c r="I139" s="44"/>
       <c r="J139" s="51"/>
@@ -40177,9 +40354,15 @@
       </c>
       <c r="C140" s="44"/>
       <c r="D140" s="44"/>
-      <c r="E140" s="44"/>
-      <c r="F140" s="44"/>
-      <c r="G140" s="44"/>
+      <c r="E140" s="44">
+        <v>0</v>
+      </c>
+      <c r="F140" s="44">
+        <v>0</v>
+      </c>
+      <c r="G140" s="44">
+        <v>0</v>
+      </c>
       <c r="H140" s="44"/>
       <c r="I140" s="44"/>
       <c r="J140" s="51"/>
@@ -40195,9 +40378,15 @@
       </c>
       <c r="C141" s="44"/>
       <c r="D141" s="44"/>
-      <c r="E141" s="44"/>
-      <c r="F141" s="44"/>
-      <c r="G141" s="44"/>
+      <c r="E141" s="44">
+        <v>0</v>
+      </c>
+      <c r="F141" s="44">
+        <v>0</v>
+      </c>
+      <c r="G141" s="44">
+        <v>0</v>
+      </c>
       <c r="H141" s="44"/>
       <c r="I141" s="44"/>
       <c r="J141" s="51"/>
@@ -40213,9 +40402,15 @@
       </c>
       <c r="C142" s="44"/>
       <c r="D142" s="44"/>
-      <c r="E142" s="44"/>
-      <c r="F142" s="44"/>
-      <c r="G142" s="44"/>
+      <c r="E142" s="44">
+        <v>0</v>
+      </c>
+      <c r="F142" s="44">
+        <v>0</v>
+      </c>
+      <c r="G142" s="44">
+        <v>0</v>
+      </c>
       <c r="H142" s="44"/>
       <c r="I142" s="44"/>
       <c r="J142" s="51"/>
@@ -40230,31 +40425,31 @@
         <v>1327</v>
       </c>
       <c r="C143" s="150">
-        <f t="shared" ref="C143:I143" si="14">SUM(C127:C142)</f>
+        <f t="shared" ref="C143:I143" si="13">SUM(C127:C142)</f>
         <v>0</v>
       </c>
       <c r="D143" s="150">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E143" s="150">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>15.14</v>
       </c>
       <c r="F143" s="150">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>15.11</v>
       </c>
       <c r="G143" s="150">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>9.16</v>
       </c>
       <c r="H143" s="150">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I143" s="150">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J143" s="51"/>
@@ -40517,31 +40712,31 @@
         <v>1368</v>
       </c>
       <c r="C156" s="150">
-        <f t="shared" ref="C156:I156" si="15">SUM(C146:C155)</f>
+        <f t="shared" ref="C156:I156" si="14">SUM(C146:C155)</f>
         <v>0</v>
       </c>
       <c r="D156" s="150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2.1887029999999998</v>
       </c>
       <c r="E156" s="150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.5424579999999999</v>
       </c>
       <c r="F156" s="150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0.42077500000000001</v>
       </c>
       <c r="G156" s="150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.3187250000000001</v>
       </c>
       <c r="H156" s="150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I156" s="150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J156" s="51"/>
@@ -66035,10 +66230,10 @@
       <c r="J317" s="69"/>
     </row>
     <row r="318" spans="1:12">
-      <c r="A318" s="233" t="s">
+      <c r="A318" s="234" t="s">
         <v>623</v>
       </c>
-      <c r="B318" s="228"/>
+      <c r="B318" s="229"/>
       <c r="C318" s="89"/>
       <c r="D318" s="89"/>
       <c r="E318" s="89"/>
@@ -66049,10 +66244,10 @@
       <c r="J318" s="69"/>
     </row>
     <row r="319" spans="1:12">
-      <c r="A319" s="232" t="s">
+      <c r="A319" s="233" t="s">
         <v>624</v>
       </c>
-      <c r="B319" s="228"/>
+      <c r="B319" s="229"/>
       <c r="C319" s="89"/>
       <c r="D319" s="89"/>
       <c r="E319" s="89"/>
@@ -66063,10 +66258,10 @@
       <c r="J319" s="69"/>
     </row>
     <row r="320" spans="1:12">
-      <c r="A320" s="232" t="s">
+      <c r="A320" s="233" t="s">
         <v>625</v>
       </c>
-      <c r="B320" s="228"/>
+      <c r="B320" s="229"/>
       <c r="C320" s="89"/>
       <c r="D320" s="89"/>
       <c r="E320" s="89"/>
@@ -66077,10 +66272,10 @@
       <c r="J320" s="69"/>
     </row>
     <row r="321" spans="1:10">
-      <c r="A321" s="232" t="s">
+      <c r="A321" s="233" t="s">
         <v>626</v>
       </c>
-      <c r="B321" s="228"/>
+      <c r="B321" s="229"/>
       <c r="C321" s="89"/>
       <c r="D321" s="89"/>
       <c r="E321" s="89"/>
@@ -66091,10 +66286,10 @@
       <c r="J321" s="69"/>
     </row>
     <row r="322" spans="1:10">
-      <c r="A322" s="232" t="s">
+      <c r="A322" s="233" t="s">
         <v>627</v>
       </c>
-      <c r="B322" s="228"/>
+      <c r="B322" s="229"/>
       <c r="C322" s="89"/>
       <c r="D322" s="89"/>
       <c r="E322" s="89"/>
@@ -66105,10 +66300,10 @@
       <c r="J322" s="69"/>
     </row>
     <row r="323" spans="1:10">
-      <c r="A323" s="232" t="s">
+      <c r="A323" s="233" t="s">
         <v>628</v>
       </c>
-      <c r="B323" s="228"/>
+      <c r="B323" s="229"/>
       <c r="C323" s="89"/>
       <c r="D323" s="89"/>
       <c r="E323" s="89"/>
@@ -66119,10 +66314,10 @@
       <c r="J323" s="69"/>
     </row>
     <row r="324" spans="1:10">
-      <c r="A324" s="232" t="s">
+      <c r="A324" s="233" t="s">
         <v>629</v>
       </c>
-      <c r="B324" s="228"/>
+      <c r="B324" s="229"/>
       <c r="C324" s="89"/>
       <c r="D324" s="89"/>
       <c r="E324" s="89"/>
@@ -66133,10 +66328,10 @@
       <c r="J324" s="69"/>
     </row>
     <row r="325" spans="1:10">
-      <c r="A325" s="232" t="s">
+      <c r="A325" s="233" t="s">
         <v>630</v>
       </c>
-      <c r="B325" s="228"/>
+      <c r="B325" s="229"/>
       <c r="C325" s="89"/>
       <c r="D325" s="89"/>
       <c r="E325" s="89"/>
@@ -66147,10 +66342,10 @@
       <c r="J325" s="69"/>
     </row>
     <row r="326" spans="1:10">
-      <c r="A326" s="232" t="s">
+      <c r="A326" s="233" t="s">
         <v>631</v>
       </c>
-      <c r="B326" s="228"/>
+      <c r="B326" s="229"/>
       <c r="C326" s="89"/>
       <c r="D326" s="89"/>
       <c r="E326" s="89"/>
@@ -66161,10 +66356,10 @@
       <c r="J326" s="69"/>
     </row>
     <row r="327" spans="1:10">
-      <c r="A327" s="232" t="s">
+      <c r="A327" s="233" t="s">
         <v>632</v>
       </c>
-      <c r="B327" s="228"/>
+      <c r="B327" s="229"/>
       <c r="C327" s="89"/>
       <c r="D327" s="89"/>
       <c r="E327" s="89"/>
@@ -66175,10 +66370,10 @@
       <c r="J327" s="69"/>
     </row>
     <row r="328" spans="1:10">
-      <c r="A328" s="232" t="s">
+      <c r="A328" s="233" t="s">
         <v>633</v>
       </c>
-      <c r="B328" s="228"/>
+      <c r="B328" s="229"/>
       <c r="C328" s="89"/>
       <c r="D328" s="89"/>
       <c r="E328" s="89"/>
@@ -66189,10 +66384,10 @@
       <c r="J328" s="69"/>
     </row>
     <row r="329" spans="1:10">
-      <c r="A329" s="232" t="s">
+      <c r="A329" s="233" t="s">
         <v>634</v>
       </c>
-      <c r="B329" s="228"/>
+      <c r="B329" s="229"/>
       <c r="C329" s="89"/>
       <c r="D329" s="89"/>
       <c r="E329" s="89"/>
@@ -66203,10 +66398,10 @@
       <c r="J329" s="69"/>
     </row>
     <row r="330" spans="1:10">
-      <c r="A330" s="232" t="s">
+      <c r="A330" s="233" t="s">
         <v>635</v>
       </c>
-      <c r="B330" s="228"/>
+      <c r="B330" s="229"/>
       <c r="C330" s="89"/>
       <c r="D330" s="89"/>
       <c r="E330" s="89"/>
@@ -66241,32 +66436,32 @@
       <c r="J332" s="69"/>
     </row>
     <row r="333" spans="1:10">
-      <c r="A333" s="235" t="s">
+      <c r="A333" s="236" t="s">
         <v>636</v>
       </c>
-      <c r="B333" s="220"/>
-      <c r="C333" s="220"/>
-      <c r="D333" s="220"/>
-      <c r="E333" s="220"/>
-      <c r="F333" s="220"/>
-      <c r="G333" s="220"/>
-      <c r="H333" s="220"/>
-      <c r="I333" s="220"/>
-      <c r="J333" s="220"/>
+      <c r="B333" s="221"/>
+      <c r="C333" s="221"/>
+      <c r="D333" s="221"/>
+      <c r="E333" s="221"/>
+      <c r="F333" s="221"/>
+      <c r="G333" s="221"/>
+      <c r="H333" s="221"/>
+      <c r="I333" s="221"/>
+      <c r="J333" s="221"/>
     </row>
     <row r="334" spans="1:10" ht="33.75" customHeight="1">
-      <c r="A334" s="234" t="s">
+      <c r="A334" s="235" t="s">
         <v>637</v>
       </c>
-      <c r="B334" s="220"/>
-      <c r="C334" s="220"/>
-      <c r="D334" s="220"/>
-      <c r="E334" s="220"/>
-      <c r="F334" s="220"/>
-      <c r="G334" s="220"/>
-      <c r="H334" s="220"/>
-      <c r="I334" s="220"/>
-      <c r="J334" s="220"/>
+      <c r="B334" s="221"/>
+      <c r="C334" s="221"/>
+      <c r="D334" s="221"/>
+      <c r="E334" s="221"/>
+      <c r="F334" s="221"/>
+      <c r="G334" s="221"/>
+      <c r="H334" s="221"/>
+      <c r="I334" s="221"/>
+      <c r="J334" s="221"/>
     </row>
     <row r="335" spans="1:10">
       <c r="A335" s="88"/>

</xml_diff>